<commit_message>
Changed to own filesystem, added armors
</commit_message>
<xml_diff>
--- a/scripts/MHW_Armor_Data.xlsx
+++ b/scripts/MHW_Armor_Data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1792" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1792" uniqueCount="461">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -949,6 +949,9 @@
     <t xml:space="preserve">159</t>
   </si>
   <si>
+    <t xml:space="preserve">Bayak Layered</t>
+  </si>
+  <si>
     <t xml:space="preserve">160</t>
   </si>
   <si>
@@ -1357,7 +1360,13 @@
     <t xml:space="preserve">244</t>
   </si>
   <si>
+    <t xml:space="preserve">Geralt A</t>
+  </si>
+  <si>
     <t xml:space="preserve">245</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ciri A</t>
   </si>
   <si>
     <t xml:space="preserve">246</t>
@@ -1626,8 +1635,8 @@
   </sheetPr>
   <dimension ref="A1:M256"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B181" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F235" activeCellId="0" sqref="B235:F235"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A241" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G246" activeCellId="0" sqref="G246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6243,22 +6252,22 @@
         <v>308</v>
       </c>
       <c r="B160" s="9" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C160" s="9" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D160" s="9" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E160" s="9" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F160" s="9" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="G160" s="8" t="s">
-        <v>21</v>
+        <v>309</v>
       </c>
       <c r="H160" s="5"/>
       <c r="I160" s="5"/>
@@ -6269,7 +6278,7 @@
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A161" s="6" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B161" s="9" t="s">
         <v>21</v>
@@ -6298,7 +6307,7 @@
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A162" s="6" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B162" s="9" t="s">
         <v>8</v>
@@ -6316,7 +6325,7 @@
         <v>21</v>
       </c>
       <c r="G162" s="8" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="H162" s="5"/>
       <c r="I162" s="5"/>
@@ -6327,7 +6336,7 @@
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A163" s="6" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B163" s="9" t="s">
         <v>8</v>
@@ -6345,7 +6354,7 @@
         <v>21</v>
       </c>
       <c r="G163" s="8" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="H163" s="5"/>
       <c r="I163" s="5"/>
@@ -6356,7 +6365,7 @@
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A164" s="6" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B164" s="9" t="s">
         <v>8</v>
@@ -6374,7 +6383,7 @@
         <v>21</v>
       </c>
       <c r="G164" s="8" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="H164" s="5"/>
       <c r="I164" s="5"/>
@@ -6385,7 +6394,7 @@
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A165" s="6" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B165" s="10" t="s">
         <v>8</v>
@@ -6403,7 +6412,7 @@
         <v>8</v>
       </c>
       <c r="G165" s="8" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="H165" s="5"/>
       <c r="I165" s="5"/>
@@ -6414,7 +6423,7 @@
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A166" s="6" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B166" s="10" t="s">
         <v>8</v>
@@ -6432,7 +6441,7 @@
         <v>8</v>
       </c>
       <c r="G166" s="8" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="H166" s="5"/>
       <c r="I166" s="5"/>
@@ -6443,7 +6452,7 @@
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A167" s="6" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B167" s="10" t="s">
         <v>8</v>
@@ -6461,7 +6470,7 @@
         <v>8</v>
       </c>
       <c r="G167" s="8" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="H167" s="5"/>
       <c r="I167" s="5"/>
@@ -6472,7 +6481,7 @@
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="6" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B168" s="9" t="s">
         <v>21</v>
@@ -6501,7 +6510,7 @@
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A169" s="6" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B169" s="9" t="s">
         <v>21</v>
@@ -6530,7 +6539,7 @@
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A170" s="6" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B170" s="7" t="s">
         <v>8</v>
@@ -6548,7 +6557,7 @@
         <v>8</v>
       </c>
       <c r="G170" s="8" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="H170" s="5"/>
       <c r="I170" s="5"/>
@@ -6559,7 +6568,7 @@
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A171" s="6" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B171" s="9" t="s">
         <v>21</v>
@@ -6588,7 +6597,7 @@
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A172" s="6" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B172" s="9" t="s">
         <v>21</v>
@@ -6617,7 +6626,7 @@
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A173" s="6" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B173" s="9" t="s">
         <v>21</v>
@@ -6646,7 +6655,7 @@
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A174" s="6" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B174" s="9" t="s">
         <v>21</v>
@@ -6675,7 +6684,7 @@
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A175" s="6" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B175" s="9" t="s">
         <v>8</v>
@@ -6693,7 +6702,7 @@
         <v>21</v>
       </c>
       <c r="G175" s="8" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="H175" s="5"/>
       <c r="I175" s="5"/>
@@ -6704,7 +6713,7 @@
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A176" s="6" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B176" s="9" t="s">
         <v>21</v>
@@ -6733,7 +6742,7 @@
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A177" s="6" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B177" s="9" t="s">
         <v>8</v>
@@ -6751,7 +6760,7 @@
         <v>21</v>
       </c>
       <c r="G177" s="8" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="H177" s="5"/>
       <c r="I177" s="5"/>
@@ -6762,7 +6771,7 @@
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A178" s="6" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B178" s="9" t="s">
         <v>21</v>
@@ -6791,7 +6800,7 @@
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A179" s="6" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B179" s="9" t="s">
         <v>8</v>
@@ -6809,7 +6818,7 @@
         <v>21</v>
       </c>
       <c r="G179" s="8" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="H179" s="5"/>
       <c r="I179" s="5"/>
@@ -6820,7 +6829,7 @@
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A180" s="6" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B180" s="9" t="s">
         <v>21</v>
@@ -6849,7 +6858,7 @@
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A181" s="6" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B181" s="9" t="s">
         <v>21</v>
@@ -6878,7 +6887,7 @@
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A182" s="6" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B182" s="9" t="s">
         <v>21</v>
@@ -6907,7 +6916,7 @@
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A183" s="6" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B183" s="9" t="s">
         <v>21</v>
@@ -6936,7 +6945,7 @@
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A184" s="6" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B184" s="9" t="s">
         <v>8</v>
@@ -6954,7 +6963,7 @@
         <v>8</v>
       </c>
       <c r="G184" s="8" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="H184" s="5"/>
       <c r="I184" s="5"/>
@@ -6965,7 +6974,7 @@
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A185" s="6" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B185" s="9" t="s">
         <v>8</v>
@@ -6983,7 +6992,7 @@
         <v>8</v>
       </c>
       <c r="G185" s="8" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="H185" s="5"/>
       <c r="I185" s="5"/>
@@ -6994,7 +7003,7 @@
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A186" s="6" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B186" s="9" t="s">
         <v>8</v>
@@ -7012,7 +7021,7 @@
         <v>8</v>
       </c>
       <c r="G186" s="8" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="H186" s="5"/>
       <c r="I186" s="5"/>
@@ -7023,7 +7032,7 @@
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A187" s="6" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B187" s="9" t="s">
         <v>8</v>
@@ -7041,7 +7050,7 @@
         <v>8</v>
       </c>
       <c r="G187" s="8" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="H187" s="5"/>
       <c r="I187" s="5"/>
@@ -7052,7 +7061,7 @@
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A188" s="6" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B188" s="9" t="s">
         <v>8</v>
@@ -7070,7 +7079,7 @@
         <v>8</v>
       </c>
       <c r="G188" s="8" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="H188" s="5"/>
       <c r="I188" s="5"/>
@@ -7081,7 +7090,7 @@
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A189" s="6" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B189" s="9" t="s">
         <v>8</v>
@@ -7099,7 +7108,7 @@
         <v>8</v>
       </c>
       <c r="G189" s="8" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="H189" s="5"/>
       <c r="I189" s="5"/>
@@ -7110,7 +7119,7 @@
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A190" s="6" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B190" s="9" t="s">
         <v>21</v>
@@ -7139,7 +7148,7 @@
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A191" s="6" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B191" s="9" t="s">
         <v>8</v>
@@ -7157,7 +7166,7 @@
         <v>8</v>
       </c>
       <c r="G191" s="8" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="H191" s="5"/>
       <c r="I191" s="5"/>
@@ -7168,7 +7177,7 @@
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A192" s="6" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B192" s="9" t="s">
         <v>8</v>
@@ -7186,7 +7195,7 @@
         <v>8</v>
       </c>
       <c r="G192" s="8" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="H192" s="5"/>
       <c r="I192" s="5"/>
@@ -7197,7 +7206,7 @@
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A193" s="6" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B193" s="9" t="s">
         <v>8</v>
@@ -7215,7 +7224,7 @@
         <v>8</v>
       </c>
       <c r="G193" s="8" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="H193" s="5"/>
       <c r="I193" s="5"/>
@@ -7226,7 +7235,7 @@
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A194" s="6" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B194" s="9" t="s">
         <v>21</v>
@@ -7255,7 +7264,7 @@
     </row>
     <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A195" s="6" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B195" s="9" t="s">
         <v>8</v>
@@ -7273,7 +7282,7 @@
         <v>8</v>
       </c>
       <c r="G195" s="8" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="H195" s="5"/>
       <c r="I195" s="5"/>
@@ -7284,7 +7293,7 @@
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A196" s="6" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B196" s="9" t="s">
         <v>8</v>
@@ -7302,7 +7311,7 @@
         <v>8</v>
       </c>
       <c r="G196" s="8" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="H196" s="5"/>
       <c r="I196" s="5"/>
@@ -7313,7 +7322,7 @@
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A197" s="6" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B197" s="9" t="s">
         <v>8</v>
@@ -7331,7 +7340,7 @@
         <v>8</v>
       </c>
       <c r="G197" s="8" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="H197" s="5"/>
       <c r="I197" s="5"/>
@@ -7342,7 +7351,7 @@
     </row>
     <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A198" s="6" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B198" s="9" t="s">
         <v>8</v>
@@ -7360,7 +7369,7 @@
         <v>8</v>
       </c>
       <c r="G198" s="8" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="H198" s="5"/>
       <c r="I198" s="5"/>
@@ -7371,7 +7380,7 @@
     </row>
     <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A199" s="6" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B199" s="9" t="s">
         <v>8</v>
@@ -7389,7 +7398,7 @@
         <v>8</v>
       </c>
       <c r="G199" s="8" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="H199" s="5"/>
       <c r="I199" s="5"/>
@@ -7400,7 +7409,7 @@
     </row>
     <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A200" s="6" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B200" s="9" t="s">
         <v>8</v>
@@ -7418,7 +7427,7 @@
         <v>8</v>
       </c>
       <c r="G200" s="8" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="H200" s="5"/>
       <c r="I200" s="5"/>
@@ -7429,7 +7438,7 @@
     </row>
     <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A201" s="6" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B201" s="9" t="s">
         <v>8</v>
@@ -7447,7 +7456,7 @@
         <v>8</v>
       </c>
       <c r="G201" s="8" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="H201" s="5"/>
       <c r="I201" s="5"/>
@@ -7458,7 +7467,7 @@
     </row>
     <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A202" s="6" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B202" s="9" t="s">
         <v>8</v>
@@ -7476,7 +7485,7 @@
         <v>8</v>
       </c>
       <c r="G202" s="8" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="H202" s="5"/>
       <c r="I202" s="5"/>
@@ -7487,7 +7496,7 @@
     </row>
     <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A203" s="6" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B203" s="11" t="s">
         <v>21</v>
@@ -7516,7 +7525,7 @@
     </row>
     <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A204" s="6" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B204" s="11" t="s">
         <v>21</v>
@@ -7545,7 +7554,7 @@
     </row>
     <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A205" s="6" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B205" s="11" t="s">
         <v>21</v>
@@ -7574,7 +7583,7 @@
     </row>
     <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A206" s="6" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B206" s="9" t="s">
         <v>8</v>
@@ -7592,7 +7601,7 @@
         <v>8</v>
       </c>
       <c r="G206" s="11" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="H206" s="5"/>
       <c r="I206" s="5"/>
@@ -7603,7 +7612,7 @@
     </row>
     <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A207" s="6" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B207" s="9" t="s">
         <v>8</v>
@@ -7621,7 +7630,7 @@
         <v>8</v>
       </c>
       <c r="G207" s="11" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="H207" s="5"/>
       <c r="I207" s="5"/>
@@ -7632,7 +7641,7 @@
     </row>
     <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A208" s="6" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B208" s="9" t="s">
         <v>8</v>
@@ -7650,7 +7659,7 @@
         <v>8</v>
       </c>
       <c r="G208" s="11" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="H208" s="5"/>
       <c r="I208" s="5"/>
@@ -7661,7 +7670,7 @@
     </row>
     <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A209" s="6" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B209" s="9" t="s">
         <v>8</v>
@@ -7679,7 +7688,7 @@
         <v>8</v>
       </c>
       <c r="G209" s="8" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="H209" s="5"/>
       <c r="I209" s="5"/>
@@ -7690,7 +7699,7 @@
     </row>
     <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A210" s="6" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B210" s="9" t="s">
         <v>8</v>
@@ -7708,7 +7717,7 @@
         <v>8</v>
       </c>
       <c r="G210" s="8" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="H210" s="5"/>
       <c r="I210" s="5"/>
@@ -7719,7 +7728,7 @@
     </row>
     <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A211" s="6" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B211" s="9" t="s">
         <v>8</v>
@@ -7737,7 +7746,7 @@
         <v>8</v>
       </c>
       <c r="G211" s="8" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="H211" s="5"/>
       <c r="I211" s="5"/>
@@ -7748,7 +7757,7 @@
     </row>
     <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A212" s="6" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B212" s="9" t="s">
         <v>8</v>
@@ -7766,7 +7775,7 @@
         <v>8</v>
       </c>
       <c r="G212" s="8" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="H212" s="5"/>
       <c r="I212" s="5"/>
@@ -7777,7 +7786,7 @@
     </row>
     <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A213" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B213" s="9" t="s">
         <v>21</v>
@@ -7806,7 +7815,7 @@
     </row>
     <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A214" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B214" s="9" t="s">
         <v>8</v>
@@ -7824,7 +7833,7 @@
         <v>8</v>
       </c>
       <c r="G214" s="8" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="H214" s="5"/>
       <c r="I214" s="5"/>
@@ -7835,7 +7844,7 @@
     </row>
     <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A215" s="6" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B215" s="9" t="s">
         <v>8</v>
@@ -7853,7 +7862,7 @@
         <v>8</v>
       </c>
       <c r="G215" s="8" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="H215" s="5"/>
       <c r="I215" s="5"/>
@@ -7864,7 +7873,7 @@
     </row>
     <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A216" s="6" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B216" s="9" t="s">
         <v>21</v>
@@ -7893,7 +7902,7 @@
     </row>
     <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A217" s="6" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B217" s="9" t="s">
         <v>21</v>
@@ -7922,7 +7931,7 @@
     </row>
     <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A218" s="6" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B218" s="9" t="s">
         <v>21</v>
@@ -7951,7 +7960,7 @@
     </row>
     <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A219" s="6" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B219" s="9" t="s">
         <v>21</v>
@@ -7980,7 +7989,7 @@
     </row>
     <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A220" s="6" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B220" s="9" t="s">
         <v>8</v>
@@ -7998,7 +8007,7 @@
         <v>8</v>
       </c>
       <c r="G220" s="8" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="H220" s="5"/>
       <c r="I220" s="5"/>
@@ -8009,7 +8018,7 @@
     </row>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A221" s="6" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B221" s="9" t="s">
         <v>8</v>
@@ -8027,7 +8036,7 @@
         <v>8</v>
       </c>
       <c r="G221" s="8" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="H221" s="5"/>
       <c r="I221" s="5"/>
@@ -8038,7 +8047,7 @@
     </row>
     <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A222" s="6" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B222" s="9" t="s">
         <v>8</v>
@@ -8056,7 +8065,7 @@
         <v>8</v>
       </c>
       <c r="G222" s="8" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="H222" s="5"/>
       <c r="I222" s="5"/>
@@ -8067,7 +8076,7 @@
     </row>
     <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A223" s="6" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B223" s="9" t="s">
         <v>8</v>
@@ -8085,7 +8094,7 @@
         <v>8</v>
       </c>
       <c r="G223" s="8" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="H223" s="5"/>
       <c r="I223" s="5"/>
@@ -8096,7 +8105,7 @@
     </row>
     <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A224" s="6" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B224" s="9" t="s">
         <v>8</v>
@@ -8114,7 +8123,7 @@
         <v>21</v>
       </c>
       <c r="G224" s="8" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="H224" s="5"/>
       <c r="I224" s="5"/>
@@ -8125,7 +8134,7 @@
     </row>
     <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A225" s="6" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B225" s="9" t="s">
         <v>8</v>
@@ -8143,7 +8152,7 @@
         <v>21</v>
       </c>
       <c r="G225" s="8" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="H225" s="5"/>
       <c r="I225" s="5"/>
@@ -8154,7 +8163,7 @@
     </row>
     <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A226" s="6" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B226" s="9" t="s">
         <v>8</v>
@@ -8172,7 +8181,7 @@
         <v>21</v>
       </c>
       <c r="G226" s="8" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="H226" s="5"/>
       <c r="I226" s="5"/>
@@ -8183,7 +8192,7 @@
     </row>
     <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A227" s="6" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B227" s="9" t="s">
         <v>8</v>
@@ -8201,7 +8210,7 @@
         <v>21</v>
       </c>
       <c r="G227" s="8" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="H227" s="5"/>
       <c r="I227" s="5"/>
@@ -8212,7 +8221,7 @@
     </row>
     <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A228" s="6" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B228" s="9" t="s">
         <v>8</v>
@@ -8230,7 +8239,7 @@
         <v>8</v>
       </c>
       <c r="G228" s="8" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="H228" s="5"/>
       <c r="I228" s="5"/>
@@ -8241,7 +8250,7 @@
     </row>
     <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A229" s="6" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B229" s="9" t="s">
         <v>8</v>
@@ -8259,7 +8268,7 @@
         <v>8</v>
       </c>
       <c r="G229" s="8" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="H229" s="5"/>
       <c r="I229" s="5"/>
@@ -8270,7 +8279,7 @@
     </row>
     <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A230" s="6" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B230" s="9" t="s">
         <v>8</v>
@@ -8288,7 +8297,7 @@
         <v>21</v>
       </c>
       <c r="G230" s="8" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="H230" s="5"/>
       <c r="I230" s="5"/>
@@ -8299,7 +8308,7 @@
     </row>
     <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A231" s="6" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B231" s="9" t="s">
         <v>21</v>
@@ -8328,7 +8337,7 @@
     </row>
     <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A232" s="6" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B232" s="9" t="s">
         <v>21</v>
@@ -8357,7 +8366,7 @@
     </row>
     <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A233" s="6" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B233" s="9" t="s">
         <v>21</v>
@@ -8386,7 +8395,7 @@
     </row>
     <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A234" s="6" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B234" s="9" t="s">
         <v>8</v>
@@ -8404,7 +8413,7 @@
         <v>21</v>
       </c>
       <c r="G234" s="8" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="H234" s="5"/>
       <c r="I234" s="5"/>
@@ -8415,7 +8424,7 @@
     </row>
     <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A235" s="6" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B235" s="9" t="s">
         <v>8</v>
@@ -8433,7 +8442,7 @@
         <v>8</v>
       </c>
       <c r="G235" s="8" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="H235" s="5"/>
       <c r="I235" s="5"/>
@@ -8444,7 +8453,7 @@
     </row>
     <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A236" s="6" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B236" s="9" t="s">
         <v>21</v>
@@ -8473,7 +8482,7 @@
     </row>
     <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A237" s="6" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B237" s="9" t="s">
         <v>21</v>
@@ -8502,7 +8511,7 @@
     </row>
     <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A238" s="6" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B238" s="9" t="s">
         <v>8</v>
@@ -8520,7 +8529,7 @@
         <v>8</v>
       </c>
       <c r="G238" s="8" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="H238" s="5"/>
       <c r="I238" s="5"/>
@@ -8531,7 +8540,7 @@
     </row>
     <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A239" s="6" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B239" s="9" t="s">
         <v>21</v>
@@ -8560,7 +8569,7 @@
     </row>
     <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A240" s="6" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="B240" s="9" t="s">
         <v>21</v>
@@ -8589,7 +8598,7 @@
     </row>
     <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A241" s="6" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B241" s="9" t="s">
         <v>21</v>
@@ -8618,7 +8627,7 @@
     </row>
     <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A242" s="6" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B242" s="9" t="s">
         <v>21</v>
@@ -8647,7 +8656,7 @@
     </row>
     <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A243" s="6" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B243" s="9" t="s">
         <v>21</v>
@@ -8676,7 +8685,7 @@
     </row>
     <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A244" s="6" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B244" s="9" t="s">
         <v>8</v>
@@ -8694,7 +8703,7 @@
         <v>8</v>
       </c>
       <c r="G244" s="8" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="H244" s="5"/>
       <c r="I244" s="5"/>
@@ -8705,25 +8714,25 @@
     </row>
     <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A245" s="6" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B245" s="9" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C245" s="9" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D245" s="9" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E245" s="9" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F245" s="9" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="G245" s="8" t="s">
-        <v>21</v>
+        <v>446</v>
       </c>
       <c r="H245" s="5"/>
       <c r="I245" s="5"/>
@@ -8734,25 +8743,25 @@
     </row>
     <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A246" s="6" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="B246" s="9" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C246" s="9" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D246" s="9" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E246" s="9" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F246" s="9" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="G246" s="8" t="s">
-        <v>21</v>
+        <v>448</v>
       </c>
       <c r="H246" s="5"/>
       <c r="I246" s="5"/>
@@ -8763,7 +8772,7 @@
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A247" s="6" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="B247" s="9" t="s">
         <v>21</v>
@@ -8792,7 +8801,7 @@
     </row>
     <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A248" s="6" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="B248" s="9" t="s">
         <v>21</v>
@@ -8821,7 +8830,7 @@
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A249" s="6" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="B249" s="9" t="s">
         <v>8</v>
@@ -8839,7 +8848,7 @@
         <v>8</v>
       </c>
       <c r="G249" s="8" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="H249" s="5"/>
       <c r="I249" s="5"/>
@@ -8850,7 +8859,7 @@
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A250" s="6" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="B250" s="9" t="s">
         <v>21</v>
@@ -8879,7 +8888,7 @@
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A251" s="6" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="B251" s="9" t="s">
         <v>21</v>
@@ -8908,7 +8917,7 @@
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A252" s="6" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="B252" s="9" t="s">
         <v>21</v>
@@ -8937,7 +8946,7 @@
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A253" s="6" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
       <c r="B253" s="12" t="s">
         <v>21</v>
@@ -8966,7 +8975,7 @@
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A254" s="6" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="B254" s="12" t="s">
         <v>8</v>
@@ -8984,7 +8993,7 @@
         <v>8</v>
       </c>
       <c r="G254" s="8" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="H254" s="5"/>
       <c r="I254" s="5"/>
@@ -8995,7 +9004,7 @@
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A255" s="6" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="B255" s="12" t="s">
         <v>21</v>
@@ -9024,7 +9033,7 @@
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A256" s="6" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="B256" s="12" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Added save sets toolbar
</commit_message>
<xml_diff>
--- a/scripts/MHW_Armor_Data.xlsx
+++ b/scripts/MHW_Armor_Data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1792" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1792" uniqueCount="462">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -1211,6 +1211,9 @@
   </si>
   <si>
     <t xml:space="preserve">212</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nergigante Y</t>
   </si>
   <si>
     <t xml:space="preserve">213</t>
@@ -1635,8 +1638,8 @@
   </sheetPr>
   <dimension ref="A1:M256"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A241" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G246" activeCellId="0" sqref="G246"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A202" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G214" activeCellId="0" sqref="G214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7789,22 +7792,22 @@
         <v>396</v>
       </c>
       <c r="B213" s="9" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C213" s="9" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D213" s="9" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E213" s="9" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F213" s="9" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="G213" s="8" t="s">
-        <v>21</v>
+        <v>397</v>
       </c>
       <c r="H213" s="5"/>
       <c r="I213" s="5"/>
@@ -7815,7 +7818,7 @@
     </row>
     <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A214" s="6" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B214" s="9" t="s">
         <v>8</v>
@@ -7833,7 +7836,7 @@
         <v>8</v>
       </c>
       <c r="G214" s="8" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="H214" s="5"/>
       <c r="I214" s="5"/>
@@ -7844,7 +7847,7 @@
     </row>
     <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A215" s="6" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B215" s="9" t="s">
         <v>8</v>
@@ -7862,7 +7865,7 @@
         <v>8</v>
       </c>
       <c r="G215" s="8" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="H215" s="5"/>
       <c r="I215" s="5"/>
@@ -7873,7 +7876,7 @@
     </row>
     <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A216" s="6" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B216" s="9" t="s">
         <v>21</v>
@@ -7902,7 +7905,7 @@
     </row>
     <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A217" s="6" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B217" s="9" t="s">
         <v>21</v>
@@ -7931,7 +7934,7 @@
     </row>
     <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A218" s="6" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B218" s="9" t="s">
         <v>21</v>
@@ -7960,7 +7963,7 @@
     </row>
     <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A219" s="6" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B219" s="9" t="s">
         <v>21</v>
@@ -7989,7 +7992,7 @@
     </row>
     <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A220" s="6" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B220" s="9" t="s">
         <v>8</v>
@@ -8007,7 +8010,7 @@
         <v>8</v>
       </c>
       <c r="G220" s="8" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="H220" s="5"/>
       <c r="I220" s="5"/>
@@ -8018,7 +8021,7 @@
     </row>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A221" s="6" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B221" s="9" t="s">
         <v>8</v>
@@ -8036,7 +8039,7 @@
         <v>8</v>
       </c>
       <c r="G221" s="8" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="H221" s="5"/>
       <c r="I221" s="5"/>
@@ -8047,7 +8050,7 @@
     </row>
     <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A222" s="6" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B222" s="9" t="s">
         <v>8</v>
@@ -8065,7 +8068,7 @@
         <v>8</v>
       </c>
       <c r="G222" s="8" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="H222" s="5"/>
       <c r="I222" s="5"/>
@@ -8076,7 +8079,7 @@
     </row>
     <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A223" s="6" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B223" s="9" t="s">
         <v>8</v>
@@ -8094,7 +8097,7 @@
         <v>8</v>
       </c>
       <c r="G223" s="8" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="H223" s="5"/>
       <c r="I223" s="5"/>
@@ -8105,7 +8108,7 @@
     </row>
     <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A224" s="6" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B224" s="9" t="s">
         <v>8</v>
@@ -8123,7 +8126,7 @@
         <v>21</v>
       </c>
       <c r="G224" s="8" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="H224" s="5"/>
       <c r="I224" s="5"/>
@@ -8134,7 +8137,7 @@
     </row>
     <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A225" s="6" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B225" s="9" t="s">
         <v>8</v>
@@ -8152,7 +8155,7 @@
         <v>21</v>
       </c>
       <c r="G225" s="8" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="H225" s="5"/>
       <c r="I225" s="5"/>
@@ -8163,7 +8166,7 @@
     </row>
     <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A226" s="6" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B226" s="9" t="s">
         <v>8</v>
@@ -8181,7 +8184,7 @@
         <v>21</v>
       </c>
       <c r="G226" s="8" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="H226" s="5"/>
       <c r="I226" s="5"/>
@@ -8192,7 +8195,7 @@
     </row>
     <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A227" s="6" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B227" s="9" t="s">
         <v>8</v>
@@ -8210,7 +8213,7 @@
         <v>21</v>
       </c>
       <c r="G227" s="8" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="H227" s="5"/>
       <c r="I227" s="5"/>
@@ -8221,7 +8224,7 @@
     </row>
     <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A228" s="6" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B228" s="9" t="s">
         <v>8</v>
@@ -8239,7 +8242,7 @@
         <v>8</v>
       </c>
       <c r="G228" s="8" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="H228" s="5"/>
       <c r="I228" s="5"/>
@@ -8250,7 +8253,7 @@
     </row>
     <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A229" s="6" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B229" s="9" t="s">
         <v>8</v>
@@ -8268,7 +8271,7 @@
         <v>8</v>
       </c>
       <c r="G229" s="8" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="H229" s="5"/>
       <c r="I229" s="5"/>
@@ -8279,7 +8282,7 @@
     </row>
     <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A230" s="6" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B230" s="9" t="s">
         <v>8</v>
@@ -8297,7 +8300,7 @@
         <v>21</v>
       </c>
       <c r="G230" s="8" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="H230" s="5"/>
       <c r="I230" s="5"/>
@@ -8308,7 +8311,7 @@
     </row>
     <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A231" s="6" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B231" s="9" t="s">
         <v>21</v>
@@ -8337,7 +8340,7 @@
     </row>
     <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A232" s="6" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B232" s="9" t="s">
         <v>21</v>
@@ -8366,7 +8369,7 @@
     </row>
     <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A233" s="6" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B233" s="9" t="s">
         <v>21</v>
@@ -8395,7 +8398,7 @@
     </row>
     <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A234" s="6" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B234" s="9" t="s">
         <v>8</v>
@@ -8413,7 +8416,7 @@
         <v>21</v>
       </c>
       <c r="G234" s="8" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="H234" s="5"/>
       <c r="I234" s="5"/>
@@ -8424,7 +8427,7 @@
     </row>
     <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A235" s="6" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="B235" s="9" t="s">
         <v>8</v>
@@ -8442,7 +8445,7 @@
         <v>8</v>
       </c>
       <c r="G235" s="8" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="H235" s="5"/>
       <c r="I235" s="5"/>
@@ -8453,7 +8456,7 @@
     </row>
     <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A236" s="6" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B236" s="9" t="s">
         <v>21</v>
@@ -8482,7 +8485,7 @@
     </row>
     <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A237" s="6" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B237" s="9" t="s">
         <v>21</v>
@@ -8511,7 +8514,7 @@
     </row>
     <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A238" s="6" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B238" s="9" t="s">
         <v>8</v>
@@ -8529,7 +8532,7 @@
         <v>8</v>
       </c>
       <c r="G238" s="8" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H238" s="5"/>
       <c r="I238" s="5"/>
@@ -8540,7 +8543,7 @@
     </row>
     <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A239" s="6" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="B239" s="9" t="s">
         <v>21</v>
@@ -8569,7 +8572,7 @@
     </row>
     <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A240" s="6" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B240" s="9" t="s">
         <v>21</v>
@@ -8598,7 +8601,7 @@
     </row>
     <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A241" s="6" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B241" s="9" t="s">
         <v>21</v>
@@ -8627,7 +8630,7 @@
     </row>
     <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A242" s="6" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B242" s="9" t="s">
         <v>21</v>
@@ -8656,7 +8659,7 @@
     </row>
     <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A243" s="6" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B243" s="9" t="s">
         <v>21</v>
@@ -8685,7 +8688,7 @@
     </row>
     <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A244" s="6" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B244" s="9" t="s">
         <v>8</v>
@@ -8703,7 +8706,7 @@
         <v>8</v>
       </c>
       <c r="G244" s="8" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="H244" s="5"/>
       <c r="I244" s="5"/>
@@ -8714,7 +8717,7 @@
     </row>
     <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A245" s="6" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="B245" s="9" t="s">
         <v>8</v>
@@ -8732,7 +8735,7 @@
         <v>8</v>
       </c>
       <c r="G245" s="8" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="H245" s="5"/>
       <c r="I245" s="5"/>
@@ -8743,7 +8746,7 @@
     </row>
     <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A246" s="6" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="B246" s="9" t="s">
         <v>8</v>
@@ -8761,7 +8764,7 @@
         <v>8</v>
       </c>
       <c r="G246" s="8" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="H246" s="5"/>
       <c r="I246" s="5"/>
@@ -8772,7 +8775,7 @@
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A247" s="6" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B247" s="9" t="s">
         <v>21</v>
@@ -8801,7 +8804,7 @@
     </row>
     <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A248" s="6" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B248" s="9" t="s">
         <v>21</v>
@@ -8830,7 +8833,7 @@
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A249" s="6" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B249" s="9" t="s">
         <v>8</v>
@@ -8848,7 +8851,7 @@
         <v>8</v>
       </c>
       <c r="G249" s="8" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="H249" s="5"/>
       <c r="I249" s="5"/>
@@ -8859,7 +8862,7 @@
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A250" s="6" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B250" s="9" t="s">
         <v>21</v>
@@ -8888,7 +8891,7 @@
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A251" s="6" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B251" s="9" t="s">
         <v>21</v>
@@ -8917,7 +8920,7 @@
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A252" s="6" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B252" s="9" t="s">
         <v>21</v>
@@ -8946,7 +8949,7 @@
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A253" s="6" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B253" s="12" t="s">
         <v>21</v>
@@ -8975,7 +8978,7 @@
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A254" s="6" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B254" s="12" t="s">
         <v>8</v>
@@ -8993,7 +8996,7 @@
         <v>8</v>
       </c>
       <c r="G254" s="8" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="H254" s="5"/>
       <c r="I254" s="5"/>
@@ -9004,7 +9007,7 @@
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A255" s="6" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="B255" s="12" t="s">
         <v>21</v>
@@ -9033,7 +9036,7 @@
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A256" s="6" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B256" s="12" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Added compatibility for game version 168030
</commit_message>
<xml_diff>
--- a/scripts/MHW_Armor_Data.xlsx
+++ b/scripts/MHW_Armor_Data.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2474" uniqueCount="1111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2476" uniqueCount="1113">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -8470,6 +8470,12 @@
   </si>
   <si>
     <t xml:space="preserve">249 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Defender α</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Defender α </t>
   </si>
   <si>
     <t xml:space="preserve">250</t>
@@ -8749,7 +8755,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -8846,6 +8852,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -8885,8 +8895,8 @@
   </sheetPr>
   <dimension ref="A1:M1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A145" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G160" activeCellId="0" sqref="G160"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A235" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J257" activeCellId="0" sqref="J257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17472,27 +17482,31 @@
         <v>1102</v>
       </c>
       <c r="B250" s="15" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="C250" s="15" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="D250" s="15" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E250" s="15" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="F250" s="16" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="G250" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H250" s="10"/>
-      <c r="I250" s="18"/>
-      <c r="J250" s="17" t="s">
-        <v>282</v>
+        <v>1103</v>
+      </c>
+      <c r="H250" s="24" t="s">
+        <v>1104</v>
+      </c>
+      <c r="I250" s="9" t="s">
+        <v>1103</v>
+      </c>
+      <c r="J250" s="9" t="s">
+        <v>1103</v>
       </c>
       <c r="K250" s="5"/>
       <c r="L250" s="5"/>
@@ -17500,7 +17514,7 @@
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A251" s="6" t="s">
-        <v>1103</v>
+        <v>1105</v>
       </c>
       <c r="B251" s="15" t="s">
         <v>40</v>
@@ -17531,7 +17545,7 @@
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A252" s="6" t="s">
-        <v>1104</v>
+        <v>1106</v>
       </c>
       <c r="B252" s="15" t="s">
         <v>40</v>
@@ -17562,9 +17576,9 @@
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A253" s="6" t="s">
-        <v>1105</v>
-      </c>
-      <c r="B253" s="24" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B253" s="25" t="s">
         <v>40</v>
       </c>
       <c r="C253" s="7" t="s">
@@ -17593,9 +17607,9 @@
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A254" s="6" t="s">
-        <v>1106</v>
-      </c>
-      <c r="B254" s="24" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B254" s="25" t="s">
         <v>11</v>
       </c>
       <c r="C254" s="7" t="s">
@@ -17611,16 +17625,16 @@
         <v>40</v>
       </c>
       <c r="G254" s="9" t="s">
-        <v>1107</v>
+        <v>1109</v>
       </c>
       <c r="H254" s="16" t="s">
-        <v>1107</v>
+        <v>1109</v>
       </c>
       <c r="I254" s="18" t="s">
-        <v>1108</v>
-      </c>
-      <c r="J254" s="17" t="s">
-        <v>282</v>
+        <v>1110</v>
+      </c>
+      <c r="J254" s="16" t="s">
+        <v>1109</v>
       </c>
       <c r="K254" s="5"/>
       <c r="L254" s="5"/>
@@ -17628,9 +17642,9 @@
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A255" s="6" t="s">
-        <v>1109</v>
-      </c>
-      <c r="B255" s="24" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B255" s="25" t="s">
         <v>40</v>
       </c>
       <c r="C255" s="7" t="s">
@@ -17659,9 +17673,9 @@
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A256" s="6" t="s">
-        <v>1110</v>
-      </c>
-      <c r="B256" s="25" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B256" s="26" t="s">
         <v>40</v>
       </c>
       <c r="C256" s="19" t="s">
@@ -17689,2437 +17703,2437 @@
       <c r="M256" s="5"/>
     </row>
     <row r="257" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G257" s="26"/>
-      <c r="J257" s="27"/>
+      <c r="G257" s="27"/>
+      <c r="J257" s="28"/>
     </row>
     <row r="258" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G258" s="26"/>
-      <c r="J258" s="27"/>
+      <c r="G258" s="27"/>
+      <c r="J258" s="28"/>
     </row>
     <row r="259" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G259" s="26"/>
-      <c r="J259" s="27"/>
+      <c r="G259" s="27"/>
+      <c r="J259" s="28"/>
     </row>
     <row r="260" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G260" s="26"/>
-      <c r="J260" s="27"/>
+      <c r="G260" s="27"/>
+      <c r="J260" s="28"/>
     </row>
     <row r="261" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G261" s="26"/>
-      <c r="J261" s="27"/>
+      <c r="G261" s="27"/>
+      <c r="J261" s="28"/>
     </row>
     <row r="262" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G262" s="26"/>
-      <c r="J262" s="27"/>
+      <c r="G262" s="27"/>
+      <c r="J262" s="28"/>
     </row>
     <row r="263" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G263" s="26"/>
-      <c r="H263" s="28"/>
-      <c r="J263" s="27"/>
+      <c r="G263" s="27"/>
+      <c r="H263" s="29"/>
+      <c r="J263" s="28"/>
     </row>
     <row r="264" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G264" s="26"/>
-      <c r="J264" s="27"/>
+      <c r="G264" s="27"/>
+      <c r="J264" s="28"/>
     </row>
     <row r="265" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G265" s="26"/>
-      <c r="J265" s="27"/>
+      <c r="G265" s="27"/>
+      <c r="J265" s="28"/>
     </row>
     <row r="266" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G266" s="26"/>
-      <c r="J266" s="27"/>
+      <c r="G266" s="27"/>
+      <c r="J266" s="28"/>
     </row>
     <row r="267" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G267" s="26"/>
-      <c r="J267" s="27"/>
+      <c r="G267" s="27"/>
+      <c r="J267" s="28"/>
     </row>
     <row r="268" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G268" s="26"/>
-      <c r="J268" s="27"/>
+      <c r="G268" s="27"/>
+      <c r="J268" s="28"/>
     </row>
     <row r="269" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G269" s="26"/>
-      <c r="J269" s="27"/>
+      <c r="G269" s="27"/>
+      <c r="J269" s="28"/>
     </row>
     <row r="270" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G270" s="26"/>
-      <c r="J270" s="27"/>
+      <c r="G270" s="27"/>
+      <c r="J270" s="28"/>
     </row>
     <row r="271" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G271" s="26"/>
-      <c r="J271" s="27"/>
+      <c r="G271" s="27"/>
+      <c r="J271" s="28"/>
     </row>
     <row r="272" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G272" s="26"/>
-      <c r="J272" s="27"/>
+      <c r="G272" s="27"/>
+      <c r="J272" s="28"/>
     </row>
     <row r="273" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G273" s="26"/>
-      <c r="J273" s="27"/>
+      <c r="G273" s="27"/>
+      <c r="J273" s="28"/>
     </row>
     <row r="274" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G274" s="26"/>
-      <c r="J274" s="27"/>
+      <c r="G274" s="27"/>
+      <c r="J274" s="28"/>
     </row>
     <row r="275" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G275" s="26"/>
-      <c r="J275" s="27"/>
+      <c r="G275" s="27"/>
+      <c r="J275" s="28"/>
     </row>
     <row r="276" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G276" s="26"/>
-      <c r="J276" s="27"/>
+      <c r="G276" s="27"/>
+      <c r="J276" s="28"/>
     </row>
     <row r="277" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G277" s="26"/>
-      <c r="J277" s="27"/>
+      <c r="G277" s="27"/>
+      <c r="J277" s="28"/>
     </row>
     <row r="278" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G278" s="26"/>
-      <c r="J278" s="27"/>
+      <c r="G278" s="27"/>
+      <c r="J278" s="28"/>
     </row>
     <row r="279" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G279" s="26"/>
-      <c r="J279" s="27"/>
+      <c r="G279" s="27"/>
+      <c r="J279" s="28"/>
     </row>
     <row r="280" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G280" s="26"/>
-      <c r="J280" s="27"/>
+      <c r="G280" s="27"/>
+      <c r="J280" s="28"/>
     </row>
     <row r="281" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G281" s="26"/>
-      <c r="J281" s="27"/>
+      <c r="G281" s="27"/>
+      <c r="J281" s="28"/>
     </row>
     <row r="282" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G282" s="26"/>
-      <c r="J282" s="27"/>
+      <c r="G282" s="27"/>
+      <c r="J282" s="28"/>
     </row>
     <row r="283" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G283" s="26"/>
-      <c r="J283" s="27"/>
+      <c r="G283" s="27"/>
+      <c r="J283" s="28"/>
     </row>
     <row r="284" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G284" s="26"/>
-      <c r="J284" s="27"/>
+      <c r="G284" s="27"/>
+      <c r="J284" s="28"/>
     </row>
     <row r="285" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G285" s="26"/>
-      <c r="J285" s="27"/>
+      <c r="G285" s="27"/>
+      <c r="J285" s="28"/>
     </row>
     <row r="286" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G286" s="26"/>
-      <c r="J286" s="27"/>
+      <c r="G286" s="27"/>
+      <c r="J286" s="28"/>
     </row>
     <row r="287" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G287" s="26"/>
-      <c r="J287" s="27"/>
+      <c r="G287" s="27"/>
+      <c r="J287" s="28"/>
     </row>
     <row r="288" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G288" s="26"/>
-      <c r="J288" s="27"/>
+      <c r="G288" s="27"/>
+      <c r="J288" s="28"/>
     </row>
     <row r="289" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G289" s="26"/>
-      <c r="J289" s="27"/>
+      <c r="G289" s="27"/>
+      <c r="J289" s="28"/>
     </row>
     <row r="290" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G290" s="26"/>
-      <c r="J290" s="27"/>
+      <c r="G290" s="27"/>
+      <c r="J290" s="28"/>
     </row>
     <row r="291" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G291" s="26"/>
-      <c r="J291" s="27"/>
+      <c r="G291" s="27"/>
+      <c r="J291" s="28"/>
     </row>
     <row r="292" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G292" s="26"/>
-      <c r="J292" s="27"/>
+      <c r="G292" s="27"/>
+      <c r="J292" s="28"/>
     </row>
     <row r="293" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G293" s="26"/>
-      <c r="J293" s="27"/>
+      <c r="G293" s="27"/>
+      <c r="J293" s="28"/>
     </row>
     <row r="294" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G294" s="26"/>
-      <c r="J294" s="27"/>
+      <c r="G294" s="27"/>
+      <c r="J294" s="28"/>
     </row>
     <row r="295" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G295" s="26"/>
-      <c r="J295" s="27"/>
+      <c r="G295" s="27"/>
+      <c r="J295" s="28"/>
     </row>
     <row r="296" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G296" s="26"/>
-      <c r="J296" s="27"/>
+      <c r="G296" s="27"/>
+      <c r="J296" s="28"/>
     </row>
     <row r="297" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G297" s="26"/>
-      <c r="J297" s="27"/>
+      <c r="G297" s="27"/>
+      <c r="J297" s="28"/>
     </row>
     <row r="298" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G298" s="26"/>
-      <c r="J298" s="27"/>
+      <c r="G298" s="27"/>
+      <c r="J298" s="28"/>
     </row>
     <row r="299" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G299" s="26"/>
-      <c r="J299" s="27"/>
+      <c r="G299" s="27"/>
+      <c r="J299" s="28"/>
     </row>
     <row r="300" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G300" s="26"/>
-      <c r="J300" s="27"/>
+      <c r="G300" s="27"/>
+      <c r="J300" s="28"/>
     </row>
     <row r="301" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G301" s="26"/>
-      <c r="J301" s="27"/>
+      <c r="G301" s="27"/>
+      <c r="J301" s="28"/>
     </row>
     <row r="302" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G302" s="26"/>
-      <c r="J302" s="27"/>
+      <c r="G302" s="27"/>
+      <c r="J302" s="28"/>
     </row>
     <row r="303" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G303" s="26"/>
-      <c r="J303" s="27"/>
+      <c r="G303" s="27"/>
+      <c r="J303" s="28"/>
     </row>
     <row r="304" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G304" s="26"/>
-      <c r="J304" s="27"/>
+      <c r="G304" s="27"/>
+      <c r="J304" s="28"/>
     </row>
     <row r="305" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G305" s="26"/>
-      <c r="J305" s="27"/>
+      <c r="G305" s="27"/>
+      <c r="J305" s="28"/>
     </row>
     <row r="306" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G306" s="26"/>
-      <c r="J306" s="27"/>
+      <c r="G306" s="27"/>
+      <c r="J306" s="28"/>
     </row>
     <row r="307" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G307" s="26"/>
-      <c r="J307" s="27"/>
+      <c r="G307" s="27"/>
+      <c r="J307" s="28"/>
     </row>
     <row r="308" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G308" s="26"/>
-      <c r="J308" s="27"/>
+      <c r="G308" s="27"/>
+      <c r="J308" s="28"/>
     </row>
     <row r="309" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G309" s="26"/>
-      <c r="J309" s="27"/>
+      <c r="G309" s="27"/>
+      <c r="J309" s="28"/>
     </row>
     <row r="310" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G310" s="26"/>
-      <c r="J310" s="27"/>
+      <c r="G310" s="27"/>
+      <c r="J310" s="28"/>
     </row>
     <row r="311" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G311" s="26"/>
-      <c r="J311" s="27"/>
+      <c r="G311" s="27"/>
+      <c r="J311" s="28"/>
     </row>
     <row r="312" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G312" s="26"/>
-      <c r="J312" s="27"/>
+      <c r="G312" s="27"/>
+      <c r="J312" s="28"/>
     </row>
     <row r="313" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G313" s="26"/>
-      <c r="J313" s="27"/>
+      <c r="G313" s="27"/>
+      <c r="J313" s="28"/>
     </row>
     <row r="314" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G314" s="26"/>
-      <c r="J314" s="27"/>
+      <c r="G314" s="27"/>
+      <c r="J314" s="28"/>
     </row>
     <row r="315" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G315" s="26"/>
-      <c r="J315" s="27"/>
+      <c r="G315" s="27"/>
+      <c r="J315" s="28"/>
     </row>
     <row r="316" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G316" s="26"/>
-      <c r="J316" s="27"/>
+      <c r="G316" s="27"/>
+      <c r="J316" s="28"/>
     </row>
     <row r="317" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G317" s="26"/>
-      <c r="J317" s="27"/>
+      <c r="G317" s="27"/>
+      <c r="J317" s="28"/>
     </row>
     <row r="318" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G318" s="26"/>
-      <c r="J318" s="27"/>
+      <c r="G318" s="27"/>
+      <c r="J318" s="28"/>
     </row>
     <row r="319" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G319" s="26"/>
-      <c r="J319" s="27"/>
+      <c r="G319" s="27"/>
+      <c r="J319" s="28"/>
     </row>
     <row r="320" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G320" s="26"/>
-      <c r="J320" s="27"/>
+      <c r="G320" s="27"/>
+      <c r="J320" s="28"/>
     </row>
     <row r="321" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G321" s="26"/>
-      <c r="J321" s="27"/>
+      <c r="G321" s="27"/>
+      <c r="J321" s="28"/>
     </row>
     <row r="322" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G322" s="26"/>
-      <c r="J322" s="27"/>
+      <c r="G322" s="27"/>
+      <c r="J322" s="28"/>
     </row>
     <row r="323" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G323" s="26"/>
-      <c r="J323" s="27"/>
+      <c r="G323" s="27"/>
+      <c r="J323" s="28"/>
     </row>
     <row r="324" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G324" s="26"/>
-      <c r="J324" s="27"/>
+      <c r="G324" s="27"/>
+      <c r="J324" s="28"/>
     </row>
     <row r="325" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G325" s="26"/>
-      <c r="J325" s="27"/>
+      <c r="G325" s="27"/>
+      <c r="J325" s="28"/>
     </row>
     <row r="326" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G326" s="26"/>
-      <c r="J326" s="27"/>
+      <c r="G326" s="27"/>
+      <c r="J326" s="28"/>
     </row>
     <row r="327" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G327" s="26"/>
-      <c r="J327" s="27"/>
+      <c r="G327" s="27"/>
+      <c r="J327" s="28"/>
     </row>
     <row r="328" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G328" s="26"/>
-      <c r="J328" s="27"/>
+      <c r="G328" s="27"/>
+      <c r="J328" s="28"/>
     </row>
     <row r="329" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G329" s="26"/>
-      <c r="J329" s="27"/>
+      <c r="G329" s="27"/>
+      <c r="J329" s="28"/>
     </row>
     <row r="330" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G330" s="26"/>
-      <c r="J330" s="27"/>
+      <c r="G330" s="27"/>
+      <c r="J330" s="28"/>
     </row>
     <row r="331" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G331" s="26"/>
-      <c r="J331" s="27"/>
+      <c r="G331" s="27"/>
+      <c r="J331" s="28"/>
     </row>
     <row r="332" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G332" s="26"/>
-      <c r="J332" s="27"/>
+      <c r="G332" s="27"/>
+      <c r="J332" s="28"/>
     </row>
     <row r="333" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G333" s="26"/>
-      <c r="J333" s="27"/>
+      <c r="G333" s="27"/>
+      <c r="J333" s="28"/>
     </row>
     <row r="334" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G334" s="26"/>
-      <c r="J334" s="27"/>
+      <c r="G334" s="27"/>
+      <c r="J334" s="28"/>
     </row>
     <row r="335" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G335" s="26"/>
-      <c r="J335" s="27"/>
+      <c r="G335" s="27"/>
+      <c r="J335" s="28"/>
     </row>
     <row r="336" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G336" s="26"/>
-      <c r="J336" s="27"/>
+      <c r="G336" s="27"/>
+      <c r="J336" s="28"/>
     </row>
     <row r="337" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G337" s="26"/>
-      <c r="J337" s="27"/>
+      <c r="G337" s="27"/>
+      <c r="J337" s="28"/>
     </row>
     <row r="338" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G338" s="26"/>
-      <c r="J338" s="27"/>
+      <c r="G338" s="27"/>
+      <c r="J338" s="28"/>
     </row>
     <row r="339" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G339" s="26"/>
-      <c r="J339" s="27"/>
+      <c r="G339" s="27"/>
+      <c r="J339" s="28"/>
     </row>
     <row r="340" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G340" s="26"/>
-      <c r="J340" s="27"/>
+      <c r="G340" s="27"/>
+      <c r="J340" s="28"/>
     </row>
     <row r="341" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G341" s="26"/>
-      <c r="J341" s="27"/>
+      <c r="G341" s="27"/>
+      <c r="J341" s="28"/>
     </row>
     <row r="342" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G342" s="26"/>
-      <c r="J342" s="27"/>
+      <c r="G342" s="27"/>
+      <c r="J342" s="28"/>
     </row>
     <row r="343" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G343" s="26"/>
-      <c r="J343" s="27"/>
+      <c r="G343" s="27"/>
+      <c r="J343" s="28"/>
     </row>
     <row r="344" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G344" s="26"/>
-      <c r="J344" s="27"/>
+      <c r="G344" s="27"/>
+      <c r="J344" s="28"/>
     </row>
     <row r="345" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G345" s="26"/>
-      <c r="J345" s="27"/>
+      <c r="G345" s="27"/>
+      <c r="J345" s="28"/>
     </row>
     <row r="346" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G346" s="26"/>
-      <c r="J346" s="27"/>
+      <c r="G346" s="27"/>
+      <c r="J346" s="28"/>
     </row>
     <row r="347" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G347" s="26"/>
-      <c r="J347" s="27"/>
+      <c r="G347" s="27"/>
+      <c r="J347" s="28"/>
     </row>
     <row r="348" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G348" s="26"/>
-      <c r="J348" s="27"/>
+      <c r="G348" s="27"/>
+      <c r="J348" s="28"/>
     </row>
     <row r="349" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G349" s="26"/>
-      <c r="J349" s="27"/>
+      <c r="G349" s="27"/>
+      <c r="J349" s="28"/>
     </row>
     <row r="350" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G350" s="26"/>
-      <c r="J350" s="27"/>
+      <c r="G350" s="27"/>
+      <c r="J350" s="28"/>
     </row>
     <row r="351" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G351" s="26"/>
-      <c r="J351" s="27"/>
+      <c r="G351" s="27"/>
+      <c r="J351" s="28"/>
     </row>
     <row r="352" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G352" s="26"/>
-      <c r="J352" s="27"/>
+      <c r="G352" s="27"/>
+      <c r="J352" s="28"/>
     </row>
     <row r="353" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G353" s="26"/>
-      <c r="J353" s="27"/>
+      <c r="G353" s="27"/>
+      <c r="J353" s="28"/>
     </row>
     <row r="354" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G354" s="26"/>
-      <c r="J354" s="27"/>
+      <c r="G354" s="27"/>
+      <c r="J354" s="28"/>
     </row>
     <row r="355" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G355" s="26"/>
-      <c r="J355" s="27"/>
+      <c r="G355" s="27"/>
+      <c r="J355" s="28"/>
     </row>
     <row r="356" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G356" s="26"/>
-      <c r="J356" s="27"/>
+      <c r="G356" s="27"/>
+      <c r="J356" s="28"/>
     </row>
     <row r="357" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G357" s="26"/>
-      <c r="J357" s="27"/>
+      <c r="G357" s="27"/>
+      <c r="J357" s="28"/>
     </row>
     <row r="358" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G358" s="26"/>
-      <c r="J358" s="27"/>
+      <c r="G358" s="27"/>
+      <c r="J358" s="28"/>
     </row>
     <row r="359" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G359" s="26"/>
-      <c r="J359" s="27"/>
+      <c r="G359" s="27"/>
+      <c r="J359" s="28"/>
     </row>
     <row r="360" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G360" s="26"/>
-      <c r="J360" s="27"/>
+      <c r="G360" s="27"/>
+      <c r="J360" s="28"/>
     </row>
     <row r="361" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G361" s="26"/>
-      <c r="J361" s="27"/>
+      <c r="G361" s="27"/>
+      <c r="J361" s="28"/>
     </row>
     <row r="362" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G362" s="26"/>
-      <c r="J362" s="27"/>
+      <c r="G362" s="27"/>
+      <c r="J362" s="28"/>
     </row>
     <row r="363" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G363" s="26"/>
-      <c r="J363" s="27"/>
+      <c r="G363" s="27"/>
+      <c r="J363" s="28"/>
     </row>
     <row r="364" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G364" s="26"/>
-      <c r="J364" s="27"/>
+      <c r="G364" s="27"/>
+      <c r="J364" s="28"/>
     </row>
     <row r="365" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G365" s="26"/>
-      <c r="J365" s="27"/>
+      <c r="G365" s="27"/>
+      <c r="J365" s="28"/>
     </row>
     <row r="366" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G366" s="26"/>
-      <c r="J366" s="27"/>
+      <c r="G366" s="27"/>
+      <c r="J366" s="28"/>
     </row>
     <row r="367" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G367" s="26"/>
-      <c r="J367" s="27"/>
+      <c r="G367" s="27"/>
+      <c r="J367" s="28"/>
     </row>
     <row r="368" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G368" s="26"/>
-      <c r="J368" s="27"/>
+      <c r="G368" s="27"/>
+      <c r="J368" s="28"/>
     </row>
     <row r="369" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G369" s="26"/>
-      <c r="J369" s="27"/>
+      <c r="G369" s="27"/>
+      <c r="J369" s="28"/>
     </row>
     <row r="370" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G370" s="26"/>
-      <c r="J370" s="27"/>
+      <c r="G370" s="27"/>
+      <c r="J370" s="28"/>
     </row>
     <row r="371" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G371" s="26"/>
-      <c r="J371" s="27"/>
+      <c r="G371" s="27"/>
+      <c r="J371" s="28"/>
     </row>
     <row r="372" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G372" s="26"/>
-      <c r="J372" s="27"/>
+      <c r="G372" s="27"/>
+      <c r="J372" s="28"/>
     </row>
     <row r="373" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G373" s="26"/>
-      <c r="J373" s="27"/>
+      <c r="G373" s="27"/>
+      <c r="J373" s="28"/>
     </row>
     <row r="374" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G374" s="26"/>
-      <c r="J374" s="27"/>
+      <c r="G374" s="27"/>
+      <c r="J374" s="28"/>
     </row>
     <row r="375" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G375" s="26"/>
-      <c r="J375" s="27"/>
+      <c r="G375" s="27"/>
+      <c r="J375" s="28"/>
     </row>
     <row r="376" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G376" s="26"/>
-      <c r="J376" s="27"/>
+      <c r="G376" s="27"/>
+      <c r="J376" s="28"/>
     </row>
     <row r="377" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G377" s="26"/>
-      <c r="J377" s="27"/>
+      <c r="G377" s="27"/>
+      <c r="J377" s="28"/>
     </row>
     <row r="378" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G378" s="26"/>
-      <c r="J378" s="27"/>
+      <c r="G378" s="27"/>
+      <c r="J378" s="28"/>
     </row>
     <row r="379" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G379" s="26"/>
-      <c r="J379" s="27"/>
+      <c r="G379" s="27"/>
+      <c r="J379" s="28"/>
     </row>
     <row r="380" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G380" s="26"/>
-      <c r="J380" s="27"/>
+      <c r="G380" s="27"/>
+      <c r="J380" s="28"/>
     </row>
     <row r="381" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G381" s="26"/>
-      <c r="J381" s="27"/>
+      <c r="G381" s="27"/>
+      <c r="J381" s="28"/>
     </row>
     <row r="382" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G382" s="26"/>
-      <c r="J382" s="27"/>
+      <c r="G382" s="27"/>
+      <c r="J382" s="28"/>
     </row>
     <row r="383" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G383" s="26"/>
-      <c r="J383" s="27"/>
+      <c r="G383" s="27"/>
+      <c r="J383" s="28"/>
     </row>
     <row r="384" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G384" s="26"/>
-      <c r="J384" s="27"/>
+      <c r="G384" s="27"/>
+      <c r="J384" s="28"/>
     </row>
     <row r="385" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G385" s="26"/>
-      <c r="J385" s="27"/>
+      <c r="G385" s="27"/>
+      <c r="J385" s="28"/>
     </row>
     <row r="386" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G386" s="26"/>
-      <c r="J386" s="27"/>
+      <c r="G386" s="27"/>
+      <c r="J386" s="28"/>
     </row>
     <row r="387" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G387" s="26"/>
-      <c r="J387" s="27"/>
+      <c r="G387" s="27"/>
+      <c r="J387" s="28"/>
     </row>
     <row r="388" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G388" s="26"/>
-      <c r="J388" s="27"/>
+      <c r="G388" s="27"/>
+      <c r="J388" s="28"/>
     </row>
     <row r="389" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G389" s="26"/>
-      <c r="J389" s="27"/>
+      <c r="G389" s="27"/>
+      <c r="J389" s="28"/>
     </row>
     <row r="390" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G390" s="26"/>
-      <c r="J390" s="27"/>
+      <c r="G390" s="27"/>
+      <c r="J390" s="28"/>
     </row>
     <row r="391" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G391" s="26"/>
-      <c r="J391" s="27"/>
+      <c r="G391" s="27"/>
+      <c r="J391" s="28"/>
     </row>
     <row r="392" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G392" s="26"/>
-      <c r="J392" s="27"/>
+      <c r="G392" s="27"/>
+      <c r="J392" s="28"/>
     </row>
     <row r="393" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G393" s="26"/>
-      <c r="J393" s="27"/>
+      <c r="G393" s="27"/>
+      <c r="J393" s="28"/>
     </row>
     <row r="394" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G394" s="26"/>
-      <c r="J394" s="27"/>
+      <c r="G394" s="27"/>
+      <c r="J394" s="28"/>
     </row>
     <row r="395" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G395" s="26"/>
-      <c r="J395" s="27"/>
+      <c r="G395" s="27"/>
+      <c r="J395" s="28"/>
     </row>
     <row r="396" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G396" s="26"/>
-      <c r="J396" s="27"/>
+      <c r="G396" s="27"/>
+      <c r="J396" s="28"/>
     </row>
     <row r="397" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G397" s="26"/>
-      <c r="J397" s="27"/>
+      <c r="G397" s="27"/>
+      <c r="J397" s="28"/>
     </row>
     <row r="398" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G398" s="26"/>
-      <c r="J398" s="27"/>
+      <c r="G398" s="27"/>
+      <c r="J398" s="28"/>
     </row>
     <row r="399" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G399" s="26"/>
-      <c r="J399" s="27"/>
+      <c r="G399" s="27"/>
+      <c r="J399" s="28"/>
     </row>
     <row r="400" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G400" s="26"/>
-      <c r="J400" s="27"/>
+      <c r="G400" s="27"/>
+      <c r="J400" s="28"/>
     </row>
     <row r="401" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G401" s="26"/>
-      <c r="J401" s="27"/>
+      <c r="G401" s="27"/>
+      <c r="J401" s="28"/>
     </row>
     <row r="402" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G402" s="26"/>
-      <c r="J402" s="27"/>
+      <c r="G402" s="27"/>
+      <c r="J402" s="28"/>
     </row>
     <row r="403" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G403" s="26"/>
-      <c r="J403" s="27"/>
+      <c r="G403" s="27"/>
+      <c r="J403" s="28"/>
     </row>
     <row r="404" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G404" s="26"/>
-      <c r="J404" s="27"/>
+      <c r="G404" s="27"/>
+      <c r="J404" s="28"/>
     </row>
     <row r="405" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G405" s="26"/>
-      <c r="J405" s="27"/>
+      <c r="G405" s="27"/>
+      <c r="J405" s="28"/>
     </row>
     <row r="406" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G406" s="26"/>
-      <c r="J406" s="27"/>
+      <c r="G406" s="27"/>
+      <c r="J406" s="28"/>
     </row>
     <row r="407" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G407" s="26"/>
-      <c r="J407" s="27"/>
+      <c r="G407" s="27"/>
+      <c r="J407" s="28"/>
     </row>
     <row r="408" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G408" s="26"/>
-      <c r="J408" s="27"/>
+      <c r="G408" s="27"/>
+      <c r="J408" s="28"/>
     </row>
     <row r="409" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G409" s="26"/>
-      <c r="J409" s="27"/>
+      <c r="G409" s="27"/>
+      <c r="J409" s="28"/>
     </row>
     <row r="410" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G410" s="26"/>
-      <c r="J410" s="27"/>
+      <c r="G410" s="27"/>
+      <c r="J410" s="28"/>
     </row>
     <row r="411" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G411" s="26"/>
-      <c r="J411" s="27"/>
+      <c r="G411" s="27"/>
+      <c r="J411" s="28"/>
     </row>
     <row r="412" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G412" s="26"/>
-      <c r="J412" s="27"/>
+      <c r="G412" s="27"/>
+      <c r="J412" s="28"/>
     </row>
     <row r="413" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G413" s="26"/>
-      <c r="J413" s="27"/>
+      <c r="G413" s="27"/>
+      <c r="J413" s="28"/>
     </row>
     <row r="414" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G414" s="26"/>
-      <c r="J414" s="27"/>
+      <c r="G414" s="27"/>
+      <c r="J414" s="28"/>
     </row>
     <row r="415" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G415" s="26"/>
-      <c r="J415" s="27"/>
+      <c r="G415" s="27"/>
+      <c r="J415" s="28"/>
     </row>
     <row r="416" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G416" s="26"/>
-      <c r="J416" s="27"/>
+      <c r="G416" s="27"/>
+      <c r="J416" s="28"/>
     </row>
     <row r="417" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G417" s="26"/>
-      <c r="J417" s="27"/>
+      <c r="G417" s="27"/>
+      <c r="J417" s="28"/>
     </row>
     <row r="418" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G418" s="26"/>
-      <c r="J418" s="27"/>
+      <c r="G418" s="27"/>
+      <c r="J418" s="28"/>
     </row>
     <row r="419" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G419" s="26"/>
-      <c r="J419" s="27"/>
+      <c r="G419" s="27"/>
+      <c r="J419" s="28"/>
     </row>
     <row r="420" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G420" s="26"/>
-      <c r="J420" s="27"/>
+      <c r="G420" s="27"/>
+      <c r="J420" s="28"/>
     </row>
     <row r="421" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G421" s="26"/>
-      <c r="J421" s="27"/>
+      <c r="G421" s="27"/>
+      <c r="J421" s="28"/>
     </row>
     <row r="422" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G422" s="26"/>
-      <c r="J422" s="27"/>
+      <c r="G422" s="27"/>
+      <c r="J422" s="28"/>
     </row>
     <row r="423" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G423" s="26"/>
-      <c r="J423" s="27"/>
+      <c r="G423" s="27"/>
+      <c r="J423" s="28"/>
     </row>
     <row r="424" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G424" s="26"/>
-      <c r="J424" s="27"/>
+      <c r="G424" s="27"/>
+      <c r="J424" s="28"/>
     </row>
     <row r="425" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G425" s="26"/>
-      <c r="J425" s="27"/>
+      <c r="G425" s="27"/>
+      <c r="J425" s="28"/>
     </row>
     <row r="426" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G426" s="26"/>
-      <c r="J426" s="27"/>
+      <c r="G426" s="27"/>
+      <c r="J426" s="28"/>
     </row>
     <row r="427" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G427" s="26"/>
-      <c r="J427" s="27"/>
+      <c r="G427" s="27"/>
+      <c r="J427" s="28"/>
     </row>
     <row r="428" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G428" s="26"/>
-      <c r="J428" s="27"/>
+      <c r="G428" s="27"/>
+      <c r="J428" s="28"/>
     </row>
     <row r="429" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G429" s="26"/>
-      <c r="J429" s="27"/>
+      <c r="G429" s="27"/>
+      <c r="J429" s="28"/>
     </row>
     <row r="430" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G430" s="26"/>
-      <c r="J430" s="27"/>
+      <c r="G430" s="27"/>
+      <c r="J430" s="28"/>
     </row>
     <row r="431" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G431" s="26"/>
-      <c r="J431" s="27"/>
+      <c r="G431" s="27"/>
+      <c r="J431" s="28"/>
     </row>
     <row r="432" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G432" s="26"/>
-      <c r="J432" s="27"/>
+      <c r="G432" s="27"/>
+      <c r="J432" s="28"/>
     </row>
     <row r="433" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G433" s="26"/>
-      <c r="J433" s="27"/>
+      <c r="G433" s="27"/>
+      <c r="J433" s="28"/>
     </row>
     <row r="434" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G434" s="26"/>
-      <c r="J434" s="27"/>
+      <c r="G434" s="27"/>
+      <c r="J434" s="28"/>
     </row>
     <row r="435" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G435" s="26"/>
-      <c r="J435" s="27"/>
+      <c r="G435" s="27"/>
+      <c r="J435" s="28"/>
     </row>
     <row r="436" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G436" s="26"/>
-      <c r="J436" s="27"/>
+      <c r="G436" s="27"/>
+      <c r="J436" s="28"/>
     </row>
     <row r="437" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G437" s="26"/>
-      <c r="J437" s="27"/>
+      <c r="G437" s="27"/>
+      <c r="J437" s="28"/>
     </row>
     <row r="438" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G438" s="26"/>
-      <c r="J438" s="27"/>
+      <c r="G438" s="27"/>
+      <c r="J438" s="28"/>
     </row>
     <row r="439" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G439" s="26"/>
-      <c r="J439" s="27"/>
+      <c r="G439" s="27"/>
+      <c r="J439" s="28"/>
     </row>
     <row r="440" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G440" s="26"/>
-      <c r="J440" s="27"/>
+      <c r="G440" s="27"/>
+      <c r="J440" s="28"/>
     </row>
     <row r="441" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G441" s="26"/>
-      <c r="J441" s="27"/>
+      <c r="G441" s="27"/>
+      <c r="J441" s="28"/>
     </row>
     <row r="442" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G442" s="26"/>
-      <c r="J442" s="27"/>
+      <c r="G442" s="27"/>
+      <c r="J442" s="28"/>
     </row>
     <row r="443" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G443" s="26"/>
-      <c r="J443" s="27"/>
+      <c r="G443" s="27"/>
+      <c r="J443" s="28"/>
     </row>
     <row r="444" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G444" s="26"/>
-      <c r="J444" s="27"/>
+      <c r="G444" s="27"/>
+      <c r="J444" s="28"/>
     </row>
     <row r="445" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G445" s="26"/>
-      <c r="J445" s="27"/>
+      <c r="G445" s="27"/>
+      <c r="J445" s="28"/>
     </row>
     <row r="446" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G446" s="26"/>
-      <c r="J446" s="27"/>
+      <c r="G446" s="27"/>
+      <c r="J446" s="28"/>
     </row>
     <row r="447" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G447" s="26"/>
-      <c r="J447" s="27"/>
+      <c r="G447" s="27"/>
+      <c r="J447" s="28"/>
     </row>
     <row r="448" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G448" s="26"/>
-      <c r="J448" s="27"/>
+      <c r="G448" s="27"/>
+      <c r="J448" s="28"/>
     </row>
     <row r="449" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G449" s="26"/>
-      <c r="J449" s="27"/>
+      <c r="G449" s="27"/>
+      <c r="J449" s="28"/>
     </row>
     <row r="450" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G450" s="26"/>
-      <c r="J450" s="27"/>
+      <c r="G450" s="27"/>
+      <c r="J450" s="28"/>
     </row>
     <row r="451" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G451" s="26"/>
-      <c r="J451" s="27"/>
+      <c r="G451" s="27"/>
+      <c r="J451" s="28"/>
     </row>
     <row r="452" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G452" s="26"/>
-      <c r="J452" s="27"/>
+      <c r="G452" s="27"/>
+      <c r="J452" s="28"/>
     </row>
     <row r="453" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G453" s="26"/>
-      <c r="J453" s="27"/>
+      <c r="G453" s="27"/>
+      <c r="J453" s="28"/>
     </row>
     <row r="454" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G454" s="26"/>
-      <c r="J454" s="27"/>
+      <c r="G454" s="27"/>
+      <c r="J454" s="28"/>
     </row>
     <row r="455" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G455" s="26"/>
-      <c r="J455" s="27"/>
+      <c r="G455" s="27"/>
+      <c r="J455" s="28"/>
     </row>
     <row r="456" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G456" s="26"/>
-      <c r="J456" s="27"/>
+      <c r="G456" s="27"/>
+      <c r="J456" s="28"/>
     </row>
     <row r="457" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J457" s="27"/>
+      <c r="J457" s="28"/>
     </row>
     <row r="458" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J458" s="27"/>
+      <c r="J458" s="28"/>
     </row>
     <row r="459" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J459" s="27"/>
+      <c r="J459" s="28"/>
     </row>
     <row r="460" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J460" s="27"/>
+      <c r="J460" s="28"/>
     </row>
     <row r="461" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J461" s="27"/>
+      <c r="J461" s="28"/>
     </row>
     <row r="462" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J462" s="27"/>
+      <c r="J462" s="28"/>
     </row>
     <row r="463" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J463" s="27"/>
+      <c r="J463" s="28"/>
     </row>
     <row r="464" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J464" s="27"/>
+      <c r="J464" s="28"/>
     </row>
     <row r="465" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J465" s="27"/>
+      <c r="J465" s="28"/>
     </row>
     <row r="466" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J466" s="27"/>
+      <c r="J466" s="28"/>
     </row>
     <row r="467" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J467" s="27"/>
+      <c r="J467" s="28"/>
     </row>
     <row r="468" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J468" s="27"/>
+      <c r="J468" s="28"/>
     </row>
     <row r="469" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J469" s="27"/>
+      <c r="J469" s="28"/>
     </row>
     <row r="470" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J470" s="27"/>
+      <c r="J470" s="28"/>
     </row>
     <row r="471" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J471" s="27"/>
+      <c r="J471" s="28"/>
     </row>
     <row r="472" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J472" s="27"/>
+      <c r="J472" s="28"/>
     </row>
     <row r="473" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J473" s="27"/>
+      <c r="J473" s="28"/>
     </row>
     <row r="474" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J474" s="27"/>
+      <c r="J474" s="28"/>
     </row>
     <row r="475" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J475" s="27"/>
+      <c r="J475" s="28"/>
     </row>
     <row r="476" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J476" s="27"/>
+      <c r="J476" s="28"/>
     </row>
     <row r="477" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J477" s="27"/>
+      <c r="J477" s="28"/>
     </row>
     <row r="478" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J478" s="27"/>
+      <c r="J478" s="28"/>
     </row>
     <row r="479" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J479" s="27"/>
+      <c r="J479" s="28"/>
     </row>
     <row r="480" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J480" s="27"/>
+      <c r="J480" s="28"/>
     </row>
     <row r="481" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J481" s="27"/>
+      <c r="J481" s="28"/>
     </row>
     <row r="482" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J482" s="27"/>
+      <c r="J482" s="28"/>
     </row>
     <row r="483" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J483" s="27"/>
+      <c r="J483" s="28"/>
     </row>
     <row r="484" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J484" s="27"/>
+      <c r="J484" s="28"/>
     </row>
     <row r="485" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J485" s="27"/>
+      <c r="J485" s="28"/>
     </row>
     <row r="486" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J486" s="27"/>
+      <c r="J486" s="28"/>
     </row>
     <row r="487" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J487" s="27"/>
+      <c r="J487" s="28"/>
     </row>
     <row r="488" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J488" s="27"/>
+      <c r="J488" s="28"/>
     </row>
     <row r="489" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J489" s="27"/>
+      <c r="J489" s="28"/>
     </row>
     <row r="490" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J490" s="27"/>
+      <c r="J490" s="28"/>
     </row>
     <row r="491" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J491" s="27"/>
+      <c r="J491" s="28"/>
     </row>
     <row r="492" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J492" s="27"/>
+      <c r="J492" s="28"/>
     </row>
     <row r="493" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J493" s="27"/>
+      <c r="J493" s="28"/>
     </row>
     <row r="494" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J494" s="27"/>
+      <c r="J494" s="28"/>
     </row>
     <row r="495" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J495" s="27"/>
+      <c r="J495" s="28"/>
     </row>
     <row r="496" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J496" s="27"/>
+      <c r="J496" s="28"/>
     </row>
     <row r="497" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J497" s="27"/>
+      <c r="J497" s="28"/>
     </row>
     <row r="498" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J498" s="27"/>
+      <c r="J498" s="28"/>
     </row>
     <row r="499" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J499" s="27"/>
+      <c r="J499" s="28"/>
     </row>
     <row r="500" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J500" s="27"/>
+      <c r="J500" s="28"/>
     </row>
     <row r="501" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J501" s="27"/>
+      <c r="J501" s="28"/>
     </row>
     <row r="502" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J502" s="27"/>
+      <c r="J502" s="28"/>
     </row>
     <row r="503" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J503" s="27"/>
+      <c r="J503" s="28"/>
     </row>
     <row r="504" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J504" s="27"/>
+      <c r="J504" s="28"/>
     </row>
     <row r="505" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J505" s="27"/>
+      <c r="J505" s="28"/>
     </row>
     <row r="506" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J506" s="27"/>
+      <c r="J506" s="28"/>
     </row>
     <row r="507" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J507" s="27"/>
+      <c r="J507" s="28"/>
     </row>
     <row r="508" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J508" s="27"/>
+      <c r="J508" s="28"/>
     </row>
     <row r="509" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J509" s="27"/>
+      <c r="J509" s="28"/>
     </row>
     <row r="510" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J510" s="27"/>
+      <c r="J510" s="28"/>
     </row>
     <row r="511" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J511" s="27"/>
+      <c r="J511" s="28"/>
     </row>
     <row r="512" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J512" s="27"/>
+      <c r="J512" s="28"/>
     </row>
     <row r="513" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J513" s="27"/>
+      <c r="J513" s="28"/>
     </row>
     <row r="514" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J514" s="27"/>
+      <c r="J514" s="28"/>
     </row>
     <row r="515" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J515" s="27"/>
+      <c r="J515" s="28"/>
     </row>
     <row r="516" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J516" s="27"/>
+      <c r="J516" s="28"/>
     </row>
     <row r="517" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J517" s="27"/>
+      <c r="J517" s="28"/>
     </row>
     <row r="518" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J518" s="27"/>
+      <c r="J518" s="28"/>
     </row>
     <row r="519" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J519" s="27"/>
+      <c r="J519" s="28"/>
     </row>
     <row r="520" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J520" s="27"/>
+      <c r="J520" s="28"/>
     </row>
     <row r="521" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J521" s="27"/>
+      <c r="J521" s="28"/>
     </row>
     <row r="522" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J522" s="27"/>
+      <c r="J522" s="28"/>
     </row>
     <row r="523" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J523" s="27"/>
+      <c r="J523" s="28"/>
     </row>
     <row r="524" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J524" s="27"/>
+      <c r="J524" s="28"/>
     </row>
     <row r="525" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J525" s="27"/>
+      <c r="J525" s="28"/>
     </row>
     <row r="526" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J526" s="27"/>
+      <c r="J526" s="28"/>
     </row>
     <row r="527" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J527" s="27"/>
+      <c r="J527" s="28"/>
     </row>
     <row r="528" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J528" s="27"/>
+      <c r="J528" s="28"/>
     </row>
     <row r="529" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J529" s="27"/>
+      <c r="J529" s="28"/>
     </row>
     <row r="530" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J530" s="27"/>
+      <c r="J530" s="28"/>
     </row>
     <row r="531" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J531" s="27"/>
+      <c r="J531" s="28"/>
     </row>
     <row r="532" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J532" s="27"/>
+      <c r="J532" s="28"/>
     </row>
     <row r="533" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J533" s="27"/>
+      <c r="J533" s="28"/>
     </row>
     <row r="534" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J534" s="27"/>
+      <c r="J534" s="28"/>
     </row>
     <row r="535" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J535" s="27"/>
+      <c r="J535" s="28"/>
     </row>
     <row r="536" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J536" s="27"/>
+      <c r="J536" s="28"/>
     </row>
     <row r="537" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J537" s="27"/>
+      <c r="J537" s="28"/>
     </row>
     <row r="538" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J538" s="27"/>
+      <c r="J538" s="28"/>
     </row>
     <row r="539" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J539" s="27"/>
+      <c r="J539" s="28"/>
     </row>
     <row r="540" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J540" s="27"/>
+      <c r="J540" s="28"/>
     </row>
     <row r="541" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J541" s="27"/>
+      <c r="J541" s="28"/>
     </row>
     <row r="542" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J542" s="27"/>
+      <c r="J542" s="28"/>
     </row>
     <row r="543" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J543" s="27"/>
+      <c r="J543" s="28"/>
     </row>
     <row r="544" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J544" s="27"/>
+      <c r="J544" s="28"/>
     </row>
     <row r="545" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J545" s="27"/>
+      <c r="J545" s="28"/>
     </row>
     <row r="546" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J546" s="27"/>
+      <c r="J546" s="28"/>
     </row>
     <row r="547" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J547" s="27"/>
+      <c r="J547" s="28"/>
     </row>
     <row r="548" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J548" s="27"/>
+      <c r="J548" s="28"/>
     </row>
     <row r="549" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J549" s="27"/>
+      <c r="J549" s="28"/>
     </row>
     <row r="550" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J550" s="27"/>
+      <c r="J550" s="28"/>
     </row>
     <row r="551" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J551" s="27"/>
+      <c r="J551" s="28"/>
     </row>
     <row r="552" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J552" s="27"/>
+      <c r="J552" s="28"/>
     </row>
     <row r="553" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J553" s="27"/>
+      <c r="J553" s="28"/>
     </row>
     <row r="554" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J554" s="27"/>
+      <c r="J554" s="28"/>
     </row>
     <row r="555" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J555" s="27"/>
+      <c r="J555" s="28"/>
     </row>
     <row r="556" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J556" s="27"/>
+      <c r="J556" s="28"/>
     </row>
     <row r="557" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J557" s="27"/>
+      <c r="J557" s="28"/>
     </row>
     <row r="558" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J558" s="27"/>
+      <c r="J558" s="28"/>
     </row>
     <row r="559" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J559" s="27"/>
+      <c r="J559" s="28"/>
     </row>
     <row r="560" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J560" s="27"/>
+      <c r="J560" s="28"/>
     </row>
     <row r="561" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J561" s="27"/>
+      <c r="J561" s="28"/>
     </row>
     <row r="562" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J562" s="27"/>
+      <c r="J562" s="28"/>
     </row>
     <row r="563" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J563" s="27"/>
+      <c r="J563" s="28"/>
     </row>
     <row r="564" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J564" s="27"/>
+      <c r="J564" s="28"/>
     </row>
     <row r="565" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J565" s="27"/>
+      <c r="J565" s="28"/>
     </row>
     <row r="566" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J566" s="27"/>
+      <c r="J566" s="28"/>
     </row>
     <row r="567" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J567" s="27"/>
+      <c r="J567" s="28"/>
     </row>
     <row r="568" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J568" s="27"/>
+      <c r="J568" s="28"/>
     </row>
     <row r="569" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J569" s="27"/>
+      <c r="J569" s="28"/>
     </row>
     <row r="570" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J570" s="27"/>
+      <c r="J570" s="28"/>
     </row>
     <row r="571" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J571" s="27"/>
+      <c r="J571" s="28"/>
     </row>
     <row r="572" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J572" s="27"/>
+      <c r="J572" s="28"/>
     </row>
     <row r="573" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J573" s="27"/>
+      <c r="J573" s="28"/>
     </row>
     <row r="574" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J574" s="27"/>
+      <c r="J574" s="28"/>
     </row>
     <row r="575" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J575" s="27"/>
+      <c r="J575" s="28"/>
     </row>
     <row r="576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J576" s="27"/>
+      <c r="J576" s="28"/>
     </row>
     <row r="577" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J577" s="27"/>
+      <c r="J577" s="28"/>
     </row>
     <row r="578" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J578" s="27"/>
+      <c r="J578" s="28"/>
     </row>
     <row r="579" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J579" s="27"/>
+      <c r="J579" s="28"/>
     </row>
     <row r="580" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J580" s="27"/>
+      <c r="J580" s="28"/>
     </row>
     <row r="581" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J581" s="27"/>
+      <c r="J581" s="28"/>
     </row>
     <row r="582" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J582" s="27"/>
+      <c r="J582" s="28"/>
     </row>
     <row r="583" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J583" s="27"/>
+      <c r="J583" s="28"/>
     </row>
     <row r="584" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J584" s="27"/>
+      <c r="J584" s="28"/>
     </row>
     <row r="585" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J585" s="27"/>
+      <c r="J585" s="28"/>
     </row>
     <row r="586" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J586" s="27"/>
+      <c r="J586" s="28"/>
     </row>
     <row r="587" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J587" s="27"/>
+      <c r="J587" s="28"/>
     </row>
     <row r="588" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J588" s="27"/>
+      <c r="J588" s="28"/>
     </row>
     <row r="589" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J589" s="27"/>
+      <c r="J589" s="28"/>
     </row>
     <row r="590" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J590" s="27"/>
+      <c r="J590" s="28"/>
     </row>
     <row r="591" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J591" s="27"/>
+      <c r="J591" s="28"/>
     </row>
     <row r="592" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J592" s="27"/>
+      <c r="J592" s="28"/>
     </row>
     <row r="593" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J593" s="27"/>
+      <c r="J593" s="28"/>
     </row>
     <row r="594" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J594" s="27"/>
+      <c r="J594" s="28"/>
     </row>
     <row r="595" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J595" s="27"/>
+      <c r="J595" s="28"/>
     </row>
     <row r="596" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J596" s="27"/>
+      <c r="J596" s="28"/>
     </row>
     <row r="597" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J597" s="27"/>
+      <c r="J597" s="28"/>
     </row>
     <row r="598" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J598" s="27"/>
+      <c r="J598" s="28"/>
     </row>
     <row r="599" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J599" s="27"/>
+      <c r="J599" s="28"/>
     </row>
     <row r="600" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J600" s="27"/>
+      <c r="J600" s="28"/>
     </row>
     <row r="601" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J601" s="27"/>
+      <c r="J601" s="28"/>
     </row>
     <row r="602" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J602" s="27"/>
+      <c r="J602" s="28"/>
     </row>
     <row r="603" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J603" s="27"/>
+      <c r="J603" s="28"/>
     </row>
     <row r="604" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J604" s="27"/>
+      <c r="J604" s="28"/>
     </row>
     <row r="605" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J605" s="27"/>
+      <c r="J605" s="28"/>
     </row>
     <row r="606" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J606" s="27"/>
+      <c r="J606" s="28"/>
     </row>
     <row r="607" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J607" s="27"/>
+      <c r="J607" s="28"/>
     </row>
     <row r="608" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J608" s="27"/>
+      <c r="J608" s="28"/>
     </row>
     <row r="609" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J609" s="27"/>
+      <c r="J609" s="28"/>
     </row>
     <row r="610" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J610" s="27"/>
+      <c r="J610" s="28"/>
     </row>
     <row r="611" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J611" s="27"/>
+      <c r="J611" s="28"/>
     </row>
     <row r="612" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J612" s="27"/>
+      <c r="J612" s="28"/>
     </row>
     <row r="613" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J613" s="27"/>
+      <c r="J613" s="28"/>
     </row>
     <row r="614" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J614" s="27"/>
+      <c r="J614" s="28"/>
     </row>
     <row r="615" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J615" s="27"/>
+      <c r="J615" s="28"/>
     </row>
     <row r="616" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J616" s="27"/>
+      <c r="J616" s="28"/>
     </row>
     <row r="617" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J617" s="27"/>
+      <c r="J617" s="28"/>
     </row>
     <row r="618" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J618" s="27"/>
+      <c r="J618" s="28"/>
     </row>
     <row r="619" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J619" s="27"/>
+      <c r="J619" s="28"/>
     </row>
     <row r="620" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J620" s="27"/>
+      <c r="J620" s="28"/>
     </row>
     <row r="621" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J621" s="27"/>
+      <c r="J621" s="28"/>
     </row>
     <row r="622" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J622" s="27"/>
+      <c r="J622" s="28"/>
     </row>
     <row r="623" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J623" s="27"/>
+      <c r="J623" s="28"/>
     </row>
     <row r="624" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J624" s="27"/>
+      <c r="J624" s="28"/>
     </row>
     <row r="625" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J625" s="27"/>
+      <c r="J625" s="28"/>
     </row>
     <row r="626" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J626" s="27"/>
+      <c r="J626" s="28"/>
     </row>
     <row r="627" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J627" s="27"/>
+      <c r="J627" s="28"/>
     </row>
     <row r="628" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J628" s="27"/>
+      <c r="J628" s="28"/>
     </row>
     <row r="629" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J629" s="27"/>
+      <c r="J629" s="28"/>
     </row>
     <row r="630" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J630" s="27"/>
+      <c r="J630" s="28"/>
     </row>
     <row r="631" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J631" s="27"/>
+      <c r="J631" s="28"/>
     </row>
     <row r="632" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J632" s="27"/>
+      <c r="J632" s="28"/>
     </row>
     <row r="633" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J633" s="27"/>
+      <c r="J633" s="28"/>
     </row>
     <row r="634" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J634" s="27"/>
+      <c r="J634" s="28"/>
     </row>
     <row r="635" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J635" s="27"/>
+      <c r="J635" s="28"/>
     </row>
     <row r="636" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J636" s="27"/>
+      <c r="J636" s="28"/>
     </row>
     <row r="637" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J637" s="27"/>
+      <c r="J637" s="28"/>
     </row>
     <row r="638" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J638" s="27"/>
+      <c r="J638" s="28"/>
     </row>
     <row r="639" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J639" s="27"/>
+      <c r="J639" s="28"/>
     </row>
     <row r="640" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J640" s="27"/>
+      <c r="J640" s="28"/>
     </row>
     <row r="641" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J641" s="27"/>
+      <c r="J641" s="28"/>
     </row>
     <row r="642" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J642" s="27"/>
+      <c r="J642" s="28"/>
     </row>
     <row r="643" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J643" s="27"/>
+      <c r="J643" s="28"/>
     </row>
     <row r="644" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J644" s="27"/>
+      <c r="J644" s="28"/>
     </row>
     <row r="645" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J645" s="27"/>
+      <c r="J645" s="28"/>
     </row>
     <row r="646" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J646" s="27"/>
+      <c r="J646" s="28"/>
     </row>
     <row r="647" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J647" s="27"/>
+      <c r="J647" s="28"/>
     </row>
     <row r="648" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J648" s="27"/>
+      <c r="J648" s="28"/>
     </row>
     <row r="649" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J649" s="27"/>
+      <c r="J649" s="28"/>
     </row>
     <row r="650" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J650" s="27"/>
+      <c r="J650" s="28"/>
     </row>
     <row r="651" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J651" s="27"/>
+      <c r="J651" s="28"/>
     </row>
     <row r="652" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J652" s="27"/>
+      <c r="J652" s="28"/>
     </row>
     <row r="653" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J653" s="27"/>
+      <c r="J653" s="28"/>
     </row>
     <row r="654" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J654" s="27"/>
+      <c r="J654" s="28"/>
     </row>
     <row r="655" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J655" s="27"/>
+      <c r="J655" s="28"/>
     </row>
     <row r="656" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J656" s="27"/>
+      <c r="J656" s="28"/>
     </row>
     <row r="657" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J657" s="27"/>
+      <c r="J657" s="28"/>
     </row>
     <row r="658" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J658" s="27"/>
+      <c r="J658" s="28"/>
     </row>
     <row r="659" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J659" s="27"/>
+      <c r="J659" s="28"/>
     </row>
     <row r="660" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J660" s="27"/>
+      <c r="J660" s="28"/>
     </row>
     <row r="661" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J661" s="27"/>
+      <c r="J661" s="28"/>
     </row>
     <row r="662" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J662" s="27"/>
+      <c r="J662" s="28"/>
     </row>
     <row r="663" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J663" s="27"/>
+      <c r="J663" s="28"/>
     </row>
     <row r="664" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J664" s="27"/>
+      <c r="J664" s="28"/>
     </row>
     <row r="665" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J665" s="27"/>
+      <c r="J665" s="28"/>
     </row>
     <row r="666" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J666" s="27"/>
+      <c r="J666" s="28"/>
     </row>
     <row r="667" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J667" s="27"/>
+      <c r="J667" s="28"/>
     </row>
     <row r="668" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J668" s="27"/>
+      <c r="J668" s="28"/>
     </row>
     <row r="669" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J669" s="27"/>
+      <c r="J669" s="28"/>
     </row>
     <row r="670" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J670" s="27"/>
+      <c r="J670" s="28"/>
     </row>
     <row r="671" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J671" s="27"/>
+      <c r="J671" s="28"/>
     </row>
     <row r="672" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J672" s="27"/>
+      <c r="J672" s="28"/>
     </row>
     <row r="673" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J673" s="27"/>
+      <c r="J673" s="28"/>
     </row>
     <row r="674" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J674" s="27"/>
+      <c r="J674" s="28"/>
     </row>
     <row r="675" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J675" s="27"/>
+      <c r="J675" s="28"/>
     </row>
     <row r="676" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J676" s="27"/>
+      <c r="J676" s="28"/>
     </row>
     <row r="677" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J677" s="27"/>
+      <c r="J677" s="28"/>
     </row>
     <row r="678" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J678" s="27"/>
+      <c r="J678" s="28"/>
     </row>
     <row r="679" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J679" s="27"/>
+      <c r="J679" s="28"/>
     </row>
     <row r="680" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J680" s="27"/>
+      <c r="J680" s="28"/>
     </row>
     <row r="681" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J681" s="27"/>
+      <c r="J681" s="28"/>
     </row>
     <row r="682" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J682" s="27"/>
+      <c r="J682" s="28"/>
     </row>
     <row r="683" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J683" s="27"/>
+      <c r="J683" s="28"/>
     </row>
     <row r="684" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J684" s="27"/>
+      <c r="J684" s="28"/>
     </row>
     <row r="685" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J685" s="27"/>
+      <c r="J685" s="28"/>
     </row>
     <row r="686" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J686" s="27"/>
+      <c r="J686" s="28"/>
     </row>
     <row r="687" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J687" s="27"/>
+      <c r="J687" s="28"/>
     </row>
     <row r="688" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J688" s="27"/>
+      <c r="J688" s="28"/>
     </row>
     <row r="689" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J689" s="27"/>
+      <c r="J689" s="28"/>
     </row>
     <row r="690" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J690" s="27"/>
+      <c r="J690" s="28"/>
     </row>
     <row r="691" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J691" s="27"/>
+      <c r="J691" s="28"/>
     </row>
     <row r="692" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J692" s="27"/>
+      <c r="J692" s="28"/>
     </row>
     <row r="693" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J693" s="27"/>
+      <c r="J693" s="28"/>
     </row>
     <row r="694" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J694" s="27"/>
+      <c r="J694" s="28"/>
     </row>
     <row r="695" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J695" s="27"/>
+      <c r="J695" s="28"/>
     </row>
     <row r="696" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J696" s="27"/>
+      <c r="J696" s="28"/>
     </row>
     <row r="697" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J697" s="27"/>
+      <c r="J697" s="28"/>
     </row>
     <row r="698" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J698" s="27"/>
+      <c r="J698" s="28"/>
     </row>
     <row r="699" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J699" s="27"/>
+      <c r="J699" s="28"/>
     </row>
     <row r="700" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J700" s="27"/>
+      <c r="J700" s="28"/>
     </row>
     <row r="701" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J701" s="27"/>
+      <c r="J701" s="28"/>
     </row>
     <row r="702" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J702" s="27"/>
+      <c r="J702" s="28"/>
     </row>
     <row r="703" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J703" s="27"/>
+      <c r="J703" s="28"/>
     </row>
     <row r="704" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J704" s="27"/>
+      <c r="J704" s="28"/>
     </row>
     <row r="705" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J705" s="27"/>
+      <c r="J705" s="28"/>
     </row>
     <row r="706" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J706" s="27"/>
+      <c r="J706" s="28"/>
     </row>
     <row r="707" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J707" s="27"/>
+      <c r="J707" s="28"/>
     </row>
     <row r="708" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J708" s="27"/>
+      <c r="J708" s="28"/>
     </row>
     <row r="709" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J709" s="27"/>
+      <c r="J709" s="28"/>
     </row>
     <row r="710" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J710" s="27"/>
+      <c r="J710" s="28"/>
     </row>
     <row r="711" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J711" s="27"/>
+      <c r="J711" s="28"/>
     </row>
     <row r="712" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J712" s="27"/>
+      <c r="J712" s="28"/>
     </row>
     <row r="713" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J713" s="27"/>
+      <c r="J713" s="28"/>
     </row>
     <row r="714" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J714" s="27"/>
+      <c r="J714" s="28"/>
     </row>
     <row r="715" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J715" s="27"/>
+      <c r="J715" s="28"/>
     </row>
     <row r="716" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J716" s="27"/>
+      <c r="J716" s="28"/>
     </row>
     <row r="717" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J717" s="27"/>
+      <c r="J717" s="28"/>
     </row>
     <row r="718" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J718" s="27"/>
+      <c r="J718" s="28"/>
     </row>
     <row r="719" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J719" s="27"/>
+      <c r="J719" s="28"/>
     </row>
     <row r="720" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J720" s="27"/>
+      <c r="J720" s="28"/>
     </row>
     <row r="721" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J721" s="27"/>
+      <c r="J721" s="28"/>
     </row>
     <row r="722" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J722" s="27"/>
+      <c r="J722" s="28"/>
     </row>
     <row r="723" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J723" s="27"/>
+      <c r="J723" s="28"/>
     </row>
     <row r="724" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J724" s="27"/>
+      <c r="J724" s="28"/>
     </row>
     <row r="725" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J725" s="27"/>
+      <c r="J725" s="28"/>
     </row>
     <row r="726" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J726" s="27"/>
+      <c r="J726" s="28"/>
     </row>
     <row r="727" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J727" s="27"/>
+      <c r="J727" s="28"/>
     </row>
     <row r="728" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J728" s="27"/>
+      <c r="J728" s="28"/>
     </row>
     <row r="729" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J729" s="27"/>
+      <c r="J729" s="28"/>
     </row>
     <row r="730" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J730" s="27"/>
+      <c r="J730" s="28"/>
     </row>
     <row r="731" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J731" s="27"/>
+      <c r="J731" s="28"/>
     </row>
     <row r="732" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J732" s="27"/>
+      <c r="J732" s="28"/>
     </row>
     <row r="733" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J733" s="27"/>
+      <c r="J733" s="28"/>
     </row>
     <row r="734" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J734" s="27"/>
+      <c r="J734" s="28"/>
     </row>
     <row r="735" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J735" s="27"/>
+      <c r="J735" s="28"/>
     </row>
     <row r="736" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J736" s="27"/>
+      <c r="J736" s="28"/>
     </row>
     <row r="737" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J737" s="27"/>
+      <c r="J737" s="28"/>
     </row>
     <row r="738" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J738" s="27"/>
+      <c r="J738" s="28"/>
     </row>
     <row r="739" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J739" s="27"/>
+      <c r="J739" s="28"/>
     </row>
     <row r="740" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J740" s="27"/>
+      <c r="J740" s="28"/>
     </row>
     <row r="741" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J741" s="27"/>
+      <c r="J741" s="28"/>
     </row>
     <row r="742" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J742" s="27"/>
+      <c r="J742" s="28"/>
     </row>
     <row r="743" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J743" s="27"/>
+      <c r="J743" s="28"/>
     </row>
     <row r="744" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J744" s="27"/>
+      <c r="J744" s="28"/>
     </row>
     <row r="745" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J745" s="27"/>
+      <c r="J745" s="28"/>
     </row>
     <row r="746" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J746" s="27"/>
+      <c r="J746" s="28"/>
     </row>
     <row r="747" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J747" s="27"/>
+      <c r="J747" s="28"/>
     </row>
     <row r="748" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J748" s="27"/>
+      <c r="J748" s="28"/>
     </row>
     <row r="749" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J749" s="27"/>
+      <c r="J749" s="28"/>
     </row>
     <row r="750" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J750" s="27"/>
+      <c r="J750" s="28"/>
     </row>
     <row r="751" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J751" s="27"/>
+      <c r="J751" s="28"/>
     </row>
     <row r="752" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J752" s="27"/>
+      <c r="J752" s="28"/>
     </row>
     <row r="753" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J753" s="27"/>
+      <c r="J753" s="28"/>
     </row>
     <row r="754" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J754" s="27"/>
+      <c r="J754" s="28"/>
     </row>
     <row r="755" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J755" s="27"/>
+      <c r="J755" s="28"/>
     </row>
     <row r="756" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J756" s="27"/>
+      <c r="J756" s="28"/>
     </row>
     <row r="757" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J757" s="27"/>
+      <c r="J757" s="28"/>
     </row>
     <row r="758" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J758" s="27"/>
+      <c r="J758" s="28"/>
     </row>
     <row r="759" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J759" s="27"/>
+      <c r="J759" s="28"/>
     </row>
     <row r="760" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J760" s="27"/>
+      <c r="J760" s="28"/>
     </row>
     <row r="761" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J761" s="27"/>
+      <c r="J761" s="28"/>
     </row>
     <row r="762" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J762" s="27"/>
+      <c r="J762" s="28"/>
     </row>
     <row r="763" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J763" s="27"/>
+      <c r="J763" s="28"/>
     </row>
     <row r="764" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J764" s="27"/>
+      <c r="J764" s="28"/>
     </row>
     <row r="765" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J765" s="27"/>
+      <c r="J765" s="28"/>
     </row>
     <row r="766" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J766" s="27"/>
+      <c r="J766" s="28"/>
     </row>
     <row r="767" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J767" s="27"/>
+      <c r="J767" s="28"/>
     </row>
     <row r="768" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J768" s="27"/>
+      <c r="J768" s="28"/>
     </row>
     <row r="769" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J769" s="27"/>
+      <c r="J769" s="28"/>
     </row>
     <row r="770" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J770" s="27"/>
+      <c r="J770" s="28"/>
     </row>
     <row r="771" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J771" s="27"/>
+      <c r="J771" s="28"/>
     </row>
     <row r="772" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J772" s="27"/>
+      <c r="J772" s="28"/>
     </row>
     <row r="773" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J773" s="27"/>
+      <c r="J773" s="28"/>
     </row>
     <row r="774" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J774" s="27"/>
+      <c r="J774" s="28"/>
     </row>
     <row r="775" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J775" s="27"/>
+      <c r="J775" s="28"/>
     </row>
     <row r="776" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J776" s="27"/>
+      <c r="J776" s="28"/>
     </row>
     <row r="777" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J777" s="27"/>
+      <c r="J777" s="28"/>
     </row>
     <row r="778" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J778" s="27"/>
+      <c r="J778" s="28"/>
     </row>
     <row r="779" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J779" s="27"/>
+      <c r="J779" s="28"/>
     </row>
     <row r="780" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J780" s="27"/>
+      <c r="J780" s="28"/>
     </row>
     <row r="781" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J781" s="27"/>
+      <c r="J781" s="28"/>
     </row>
     <row r="782" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J782" s="27"/>
+      <c r="J782" s="28"/>
     </row>
     <row r="783" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J783" s="27"/>
+      <c r="J783" s="28"/>
     </row>
     <row r="784" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J784" s="27"/>
+      <c r="J784" s="28"/>
     </row>
     <row r="785" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J785" s="27"/>
+      <c r="J785" s="28"/>
     </row>
     <row r="786" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J786" s="27"/>
+      <c r="J786" s="28"/>
     </row>
     <row r="787" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J787" s="27"/>
+      <c r="J787" s="28"/>
     </row>
     <row r="788" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J788" s="27"/>
+      <c r="J788" s="28"/>
     </row>
     <row r="789" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J789" s="27"/>
+      <c r="J789" s="28"/>
     </row>
     <row r="790" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J790" s="27"/>
+      <c r="J790" s="28"/>
     </row>
     <row r="791" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J791" s="27"/>
+      <c r="J791" s="28"/>
     </row>
     <row r="792" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J792" s="27"/>
+      <c r="J792" s="28"/>
     </row>
     <row r="793" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J793" s="27"/>
+      <c r="J793" s="28"/>
     </row>
     <row r="794" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J794" s="27"/>
+      <c r="J794" s="28"/>
     </row>
     <row r="795" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J795" s="27"/>
+      <c r="J795" s="28"/>
     </row>
     <row r="796" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J796" s="27"/>
+      <c r="J796" s="28"/>
     </row>
     <row r="797" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J797" s="27"/>
+      <c r="J797" s="28"/>
     </row>
     <row r="798" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J798" s="27"/>
+      <c r="J798" s="28"/>
     </row>
     <row r="799" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J799" s="27"/>
+      <c r="J799" s="28"/>
     </row>
     <row r="800" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J800" s="27"/>
+      <c r="J800" s="28"/>
     </row>
     <row r="801" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J801" s="27"/>
+      <c r="J801" s="28"/>
     </row>
     <row r="802" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J802" s="27"/>
+      <c r="J802" s="28"/>
     </row>
     <row r="803" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J803" s="27"/>
+      <c r="J803" s="28"/>
     </row>
     <row r="804" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J804" s="27"/>
+      <c r="J804" s="28"/>
     </row>
     <row r="805" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J805" s="27"/>
+      <c r="J805" s="28"/>
     </row>
     <row r="806" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J806" s="27"/>
+      <c r="J806" s="28"/>
     </row>
     <row r="807" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J807" s="27"/>
+      <c r="J807" s="28"/>
     </row>
     <row r="808" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J808" s="27"/>
+      <c r="J808" s="28"/>
     </row>
     <row r="809" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J809" s="27"/>
+      <c r="J809" s="28"/>
     </row>
     <row r="810" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J810" s="27"/>
+      <c r="J810" s="28"/>
     </row>
     <row r="811" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J811" s="27"/>
+      <c r="J811" s="28"/>
     </row>
     <row r="812" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J812" s="27"/>
+      <c r="J812" s="28"/>
     </row>
     <row r="813" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J813" s="27"/>
+      <c r="J813" s="28"/>
     </row>
     <row r="814" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J814" s="27"/>
+      <c r="J814" s="28"/>
     </row>
     <row r="815" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J815" s="27"/>
+      <c r="J815" s="28"/>
     </row>
     <row r="816" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J816" s="27"/>
+      <c r="J816" s="28"/>
     </row>
     <row r="817" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J817" s="27"/>
+      <c r="J817" s="28"/>
     </row>
     <row r="818" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J818" s="27"/>
+      <c r="J818" s="28"/>
     </row>
     <row r="819" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J819" s="27"/>
+      <c r="J819" s="28"/>
     </row>
     <row r="820" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J820" s="27"/>
+      <c r="J820" s="28"/>
     </row>
     <row r="821" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J821" s="27"/>
+      <c r="J821" s="28"/>
     </row>
     <row r="822" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J822" s="27"/>
+      <c r="J822" s="28"/>
     </row>
     <row r="823" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J823" s="27"/>
+      <c r="J823" s="28"/>
     </row>
     <row r="824" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J824" s="27"/>
+      <c r="J824" s="28"/>
     </row>
     <row r="825" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J825" s="27"/>
+      <c r="J825" s="28"/>
     </row>
     <row r="826" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J826" s="27"/>
+      <c r="J826" s="28"/>
     </row>
     <row r="827" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J827" s="27"/>
+      <c r="J827" s="28"/>
     </row>
     <row r="828" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J828" s="27"/>
+      <c r="J828" s="28"/>
     </row>
     <row r="829" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J829" s="27"/>
+      <c r="J829" s="28"/>
     </row>
     <row r="830" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J830" s="27"/>
+      <c r="J830" s="28"/>
     </row>
     <row r="831" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J831" s="27"/>
+      <c r="J831" s="28"/>
     </row>
     <row r="832" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J832" s="27"/>
+      <c r="J832" s="28"/>
     </row>
     <row r="833" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J833" s="27"/>
+      <c r="J833" s="28"/>
     </row>
     <row r="834" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J834" s="27"/>
+      <c r="J834" s="28"/>
     </row>
     <row r="835" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J835" s="27"/>
+      <c r="J835" s="28"/>
     </row>
     <row r="836" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J836" s="27"/>
+      <c r="J836" s="28"/>
     </row>
     <row r="837" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J837" s="27"/>
+      <c r="J837" s="28"/>
     </row>
     <row r="838" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J838" s="27"/>
+      <c r="J838" s="28"/>
     </row>
     <row r="839" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J839" s="27"/>
+      <c r="J839" s="28"/>
     </row>
     <row r="840" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J840" s="27"/>
+      <c r="J840" s="28"/>
     </row>
     <row r="841" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J841" s="27"/>
+      <c r="J841" s="28"/>
     </row>
     <row r="842" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J842" s="27"/>
+      <c r="J842" s="28"/>
     </row>
     <row r="843" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J843" s="27"/>
+      <c r="J843" s="28"/>
     </row>
     <row r="844" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J844" s="27"/>
+      <c r="J844" s="28"/>
     </row>
     <row r="845" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J845" s="27"/>
+      <c r="J845" s="28"/>
     </row>
     <row r="846" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J846" s="27"/>
+      <c r="J846" s="28"/>
     </row>
     <row r="847" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J847" s="27"/>
+      <c r="J847" s="28"/>
     </row>
     <row r="848" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J848" s="27"/>
+      <c r="J848" s="28"/>
     </row>
     <row r="849" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J849" s="27"/>
+      <c r="J849" s="28"/>
     </row>
     <row r="850" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J850" s="27"/>
+      <c r="J850" s="28"/>
     </row>
     <row r="851" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J851" s="27"/>
+      <c r="J851" s="28"/>
     </row>
     <row r="852" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J852" s="27"/>
+      <c r="J852" s="28"/>
     </row>
     <row r="853" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J853" s="27"/>
+      <c r="J853" s="28"/>
     </row>
     <row r="854" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J854" s="27"/>
+      <c r="J854" s="28"/>
     </row>
     <row r="855" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J855" s="27"/>
+      <c r="J855" s="28"/>
     </row>
     <row r="856" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J856" s="27"/>
+      <c r="J856" s="28"/>
     </row>
     <row r="857" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J857" s="27"/>
+      <c r="J857" s="28"/>
     </row>
     <row r="858" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J858" s="27"/>
+      <c r="J858" s="28"/>
     </row>
     <row r="859" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J859" s="27"/>
+      <c r="J859" s="28"/>
     </row>
     <row r="860" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J860" s="27"/>
+      <c r="J860" s="28"/>
     </row>
     <row r="861" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J861" s="27"/>
+      <c r="J861" s="28"/>
     </row>
     <row r="862" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J862" s="27"/>
+      <c r="J862" s="28"/>
     </row>
     <row r="863" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J863" s="27"/>
+      <c r="J863" s="28"/>
     </row>
     <row r="864" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J864" s="27"/>
+      <c r="J864" s="28"/>
     </row>
     <row r="865" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J865" s="27"/>
+      <c r="J865" s="28"/>
     </row>
     <row r="866" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J866" s="27"/>
+      <c r="J866" s="28"/>
     </row>
     <row r="867" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J867" s="27"/>
+      <c r="J867" s="28"/>
     </row>
     <row r="868" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J868" s="27"/>
+      <c r="J868" s="28"/>
     </row>
     <row r="869" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J869" s="27"/>
+      <c r="J869" s="28"/>
     </row>
     <row r="870" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J870" s="27"/>
+      <c r="J870" s="28"/>
     </row>
     <row r="871" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J871" s="27"/>
+      <c r="J871" s="28"/>
     </row>
     <row r="872" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J872" s="27"/>
+      <c r="J872" s="28"/>
     </row>
     <row r="873" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J873" s="27"/>
+      <c r="J873" s="28"/>
     </row>
     <row r="874" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J874" s="27"/>
+      <c r="J874" s="28"/>
     </row>
     <row r="875" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J875" s="27"/>
+      <c r="J875" s="28"/>
     </row>
     <row r="876" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J876" s="27"/>
+      <c r="J876" s="28"/>
     </row>
     <row r="877" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J877" s="27"/>
+      <c r="J877" s="28"/>
     </row>
     <row r="878" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J878" s="27"/>
+      <c r="J878" s="28"/>
     </row>
     <row r="879" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J879" s="27"/>
+      <c r="J879" s="28"/>
     </row>
     <row r="880" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J880" s="27"/>
+      <c r="J880" s="28"/>
     </row>
     <row r="881" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J881" s="27"/>
+      <c r="J881" s="28"/>
     </row>
     <row r="882" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J882" s="27"/>
+      <c r="J882" s="28"/>
     </row>
     <row r="883" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J883" s="27"/>
+      <c r="J883" s="28"/>
     </row>
     <row r="884" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J884" s="27"/>
+      <c r="J884" s="28"/>
     </row>
     <row r="885" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J885" s="27"/>
+      <c r="J885" s="28"/>
     </row>
     <row r="886" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J886" s="27"/>
+      <c r="J886" s="28"/>
     </row>
     <row r="887" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J887" s="27"/>
+      <c r="J887" s="28"/>
     </row>
     <row r="888" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J888" s="27"/>
+      <c r="J888" s="28"/>
     </row>
     <row r="889" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J889" s="27"/>
+      <c r="J889" s="28"/>
     </row>
     <row r="890" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J890" s="27"/>
+      <c r="J890" s="28"/>
     </row>
     <row r="891" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J891" s="27"/>
+      <c r="J891" s="28"/>
     </row>
     <row r="892" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J892" s="27"/>
+      <c r="J892" s="28"/>
     </row>
     <row r="893" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J893" s="27"/>
+      <c r="J893" s="28"/>
     </row>
     <row r="894" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J894" s="27"/>
+      <c r="J894" s="28"/>
     </row>
     <row r="895" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J895" s="27"/>
+      <c r="J895" s="28"/>
     </row>
     <row r="896" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J896" s="27"/>
+      <c r="J896" s="28"/>
     </row>
     <row r="897" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J897" s="27"/>
+      <c r="J897" s="28"/>
     </row>
     <row r="898" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J898" s="27"/>
+      <c r="J898" s="28"/>
     </row>
     <row r="899" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J899" s="27"/>
+      <c r="J899" s="28"/>
     </row>
     <row r="900" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J900" s="27"/>
+      <c r="J900" s="28"/>
     </row>
     <row r="901" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J901" s="27"/>
+      <c r="J901" s="28"/>
     </row>
     <row r="902" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J902" s="27"/>
+      <c r="J902" s="28"/>
     </row>
     <row r="903" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J903" s="27"/>
+      <c r="J903" s="28"/>
     </row>
     <row r="904" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J904" s="27"/>
+      <c r="J904" s="28"/>
     </row>
     <row r="905" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J905" s="27"/>
+      <c r="J905" s="28"/>
     </row>
     <row r="906" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J906" s="27"/>
+      <c r="J906" s="28"/>
     </row>
     <row r="907" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J907" s="27"/>
+      <c r="J907" s="28"/>
     </row>
     <row r="908" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J908" s="27"/>
+      <c r="J908" s="28"/>
     </row>
     <row r="909" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J909" s="27"/>
+      <c r="J909" s="28"/>
     </row>
     <row r="910" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J910" s="27"/>
+      <c r="J910" s="28"/>
     </row>
     <row r="911" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J911" s="27"/>
+      <c r="J911" s="28"/>
     </row>
     <row r="912" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J912" s="27"/>
+      <c r="J912" s="28"/>
     </row>
     <row r="913" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J913" s="27"/>
+      <c r="J913" s="28"/>
     </row>
     <row r="914" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J914" s="27"/>
+      <c r="J914" s="28"/>
     </row>
     <row r="915" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J915" s="27"/>
+      <c r="J915" s="28"/>
     </row>
     <row r="916" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J916" s="27"/>
+      <c r="J916" s="28"/>
     </row>
     <row r="917" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J917" s="27"/>
+      <c r="J917" s="28"/>
     </row>
     <row r="918" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J918" s="27"/>
+      <c r="J918" s="28"/>
     </row>
     <row r="919" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J919" s="27"/>
+      <c r="J919" s="28"/>
     </row>
     <row r="920" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J920" s="27"/>
+      <c r="J920" s="28"/>
     </row>
     <row r="921" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J921" s="27"/>
+      <c r="J921" s="28"/>
     </row>
     <row r="922" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J922" s="27"/>
+      <c r="J922" s="28"/>
     </row>
     <row r="923" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J923" s="27"/>
+      <c r="J923" s="28"/>
     </row>
     <row r="924" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J924" s="27"/>
+      <c r="J924" s="28"/>
     </row>
     <row r="925" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J925" s="27"/>
+      <c r="J925" s="28"/>
     </row>
     <row r="926" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J926" s="27"/>
+      <c r="J926" s="28"/>
     </row>
     <row r="927" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J927" s="27"/>
+      <c r="J927" s="28"/>
     </row>
     <row r="928" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J928" s="27"/>
+      <c r="J928" s="28"/>
     </row>
     <row r="929" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J929" s="27"/>
+      <c r="J929" s="28"/>
     </row>
     <row r="930" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J930" s="27"/>
+      <c r="J930" s="28"/>
     </row>
     <row r="931" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J931" s="27"/>
+      <c r="J931" s="28"/>
     </row>
     <row r="932" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J932" s="27"/>
+      <c r="J932" s="28"/>
     </row>
     <row r="933" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J933" s="27"/>
+      <c r="J933" s="28"/>
     </row>
     <row r="934" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J934" s="27"/>
+      <c r="J934" s="28"/>
     </row>
     <row r="935" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J935" s="27"/>
+      <c r="J935" s="28"/>
     </row>
     <row r="936" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J936" s="27"/>
+      <c r="J936" s="28"/>
     </row>
     <row r="937" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J937" s="27"/>
+      <c r="J937" s="28"/>
     </row>
     <row r="938" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J938" s="27"/>
+      <c r="J938" s="28"/>
     </row>
     <row r="939" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J939" s="27"/>
+      <c r="J939" s="28"/>
     </row>
     <row r="940" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J940" s="27"/>
+      <c r="J940" s="28"/>
     </row>
     <row r="941" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J941" s="27"/>
+      <c r="J941" s="28"/>
     </row>
     <row r="942" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J942" s="27"/>
+      <c r="J942" s="28"/>
     </row>
     <row r="943" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J943" s="27"/>
+      <c r="J943" s="28"/>
     </row>
     <row r="944" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J944" s="27"/>
+      <c r="J944" s="28"/>
     </row>
     <row r="945" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J945" s="27"/>
+      <c r="J945" s="28"/>
     </row>
     <row r="946" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J946" s="27"/>
+      <c r="J946" s="28"/>
     </row>
     <row r="947" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J947" s="27"/>
+      <c r="J947" s="28"/>
     </row>
     <row r="948" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J948" s="27"/>
+      <c r="J948" s="28"/>
     </row>
     <row r="949" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J949" s="27"/>
+      <c r="J949" s="28"/>
     </row>
     <row r="950" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J950" s="27"/>
+      <c r="J950" s="28"/>
     </row>
     <row r="951" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J951" s="27"/>
+      <c r="J951" s="28"/>
     </row>
     <row r="952" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J952" s="27"/>
+      <c r="J952" s="28"/>
     </row>
     <row r="953" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J953" s="27"/>
+      <c r="J953" s="28"/>
     </row>
     <row r="954" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J954" s="27"/>
+      <c r="J954" s="28"/>
     </row>
     <row r="955" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J955" s="27"/>
+      <c r="J955" s="28"/>
     </row>
     <row r="956" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J956" s="27"/>
+      <c r="J956" s="28"/>
     </row>
     <row r="957" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J957" s="27"/>
+      <c r="J957" s="28"/>
     </row>
     <row r="958" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J958" s="27"/>
+      <c r="J958" s="28"/>
     </row>
     <row r="959" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J959" s="27"/>
+      <c r="J959" s="28"/>
     </row>
     <row r="960" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J960" s="27"/>
+      <c r="J960" s="28"/>
     </row>
     <row r="961" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J961" s="27"/>
+      <c r="J961" s="28"/>
     </row>
     <row r="962" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J962" s="27"/>
+      <c r="J962" s="28"/>
     </row>
     <row r="963" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J963" s="27"/>
+      <c r="J963" s="28"/>
     </row>
     <row r="964" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J964" s="27"/>
+      <c r="J964" s="28"/>
     </row>
     <row r="965" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J965" s="27"/>
+      <c r="J965" s="28"/>
     </row>
     <row r="966" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J966" s="27"/>
+      <c r="J966" s="28"/>
     </row>
     <row r="967" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J967" s="27"/>
+      <c r="J967" s="28"/>
     </row>
     <row r="968" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J968" s="27"/>
+      <c r="J968" s="28"/>
     </row>
     <row r="969" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J969" s="27"/>
+      <c r="J969" s="28"/>
     </row>
     <row r="970" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J970" s="27"/>
+      <c r="J970" s="28"/>
     </row>
     <row r="971" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J971" s="27"/>
+      <c r="J971" s="28"/>
     </row>
     <row r="972" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J972" s="27"/>
+      <c r="J972" s="28"/>
     </row>
     <row r="973" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J973" s="27"/>
+      <c r="J973" s="28"/>
     </row>
     <row r="974" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J974" s="27"/>
+      <c r="J974" s="28"/>
     </row>
     <row r="975" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J975" s="27"/>
+      <c r="J975" s="28"/>
     </row>
     <row r="976" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J976" s="27"/>
+      <c r="J976" s="28"/>
     </row>
     <row r="977" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J977" s="27"/>
+      <c r="J977" s="28"/>
     </row>
     <row r="978" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J978" s="27"/>
+      <c r="J978" s="28"/>
     </row>
     <row r="979" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J979" s="27"/>
+      <c r="J979" s="28"/>
     </row>
     <row r="980" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J980" s="27"/>
+      <c r="J980" s="28"/>
     </row>
     <row r="981" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J981" s="27"/>
+      <c r="J981" s="28"/>
     </row>
     <row r="982" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J982" s="27"/>
+      <c r="J982" s="28"/>
     </row>
     <row r="983" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J983" s="27"/>
+      <c r="J983" s="28"/>
     </row>
     <row r="984" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J984" s="27"/>
+      <c r="J984" s="28"/>
     </row>
     <row r="985" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J985" s="27"/>
+      <c r="J985" s="28"/>
     </row>
     <row r="986" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J986" s="27"/>
+      <c r="J986" s="28"/>
     </row>
     <row r="987" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J987" s="27"/>
+      <c r="J987" s="28"/>
     </row>
     <row r="988" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J988" s="27"/>
+      <c r="J988" s="28"/>
     </row>
     <row r="989" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J989" s="27"/>
+      <c r="J989" s="28"/>
     </row>
     <row r="990" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J990" s="27"/>
+      <c r="J990" s="28"/>
     </row>
     <row r="991" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J991" s="27"/>
+      <c r="J991" s="28"/>
     </row>
     <row r="992" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J992" s="27"/>
+      <c r="J992" s="28"/>
     </row>
     <row r="993" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J993" s="27"/>
+      <c r="J993" s="28"/>
     </row>
     <row r="994" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J994" s="27"/>
+      <c r="J994" s="28"/>
     </row>
     <row r="995" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J995" s="27"/>
+      <c r="J995" s="28"/>
     </row>
     <row r="996" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J996" s="27"/>
+      <c r="J996" s="28"/>
     </row>
     <row r="997" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J997" s="27"/>
+      <c r="J997" s="28"/>
     </row>
     <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J998" s="27"/>
+      <c r="J998" s="28"/>
     </row>
     <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J999" s="27"/>
+      <c r="J999" s="28"/>
     </row>
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J1000" s="27"/>
+      <c r="J1000" s="28"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Lots of changes, see CHANGELOG
</commit_message>
<xml_diff>
--- a/scripts/MHW_Armor_Data.xlsx
+++ b/scripts/MHW_Armor_Data.xlsx
@@ -15097,8 +15097,8 @@
   </sheetPr>
   <dimension ref="A1:M1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A460" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I467" activeCellId="0" sqref="I467"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A355" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G368" activeCellId="0" sqref="G368"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Added Compatibility with game version 402862
</commit_message>
<xml_diff>
--- a/scripts/MHW_Armor_Data.xlsx
+++ b/scripts/MHW_Armor_Data.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4758" uniqueCount="1698">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4764" uniqueCount="1700">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -14013,7 +14013,59 @@
     <t xml:space="preserve">428</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Rajang </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">α+</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">429</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Rajang </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">β</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">430</t>
@@ -14709,7 +14761,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -14846,6 +14898,12 @@
       <name val="돋움"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -15074,7 +15132,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -15097,8 +15155,8 @@
   </sheetPr>
   <dimension ref="A1:M1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A355" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G368" activeCellId="0" sqref="G368"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A421" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F430" activeCellId="0" sqref="F430"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29011,57 +29069,69 @@
       <c r="A429" s="6" t="s">
         <v>1580</v>
       </c>
-      <c r="B429" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C429" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D429" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="E429" s="15" t="s">
-        <v>40</v>
+      <c r="B429" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C429" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D429" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E429" s="16" t="s">
+        <v>11</v>
       </c>
       <c r="F429" s="16" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="G429" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H429" s="10"/>
-      <c r="I429" s="20"/>
-      <c r="J429" s="19"/>
+        <v>1581</v>
+      </c>
+      <c r="H429" s="9" t="s">
+        <v>1581</v>
+      </c>
+      <c r="I429" s="9" t="s">
+        <v>1581</v>
+      </c>
+      <c r="J429" s="9" t="s">
+        <v>1581</v>
+      </c>
     </row>
     <row r="430" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A430" s="6" t="s">
-        <v>1581</v>
-      </c>
-      <c r="B430" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C430" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D430" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="E430" s="15" t="s">
-        <v>40</v>
+        <v>1582</v>
+      </c>
+      <c r="B430" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C430" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D430" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E430" s="16" t="s">
+        <v>11</v>
       </c>
       <c r="F430" s="16" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="G430" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H430" s="10"/>
-      <c r="I430" s="20"/>
-      <c r="J430" s="19"/>
+        <v>1583</v>
+      </c>
+      <c r="H430" s="9" t="s">
+        <v>1583</v>
+      </c>
+      <c r="I430" s="9" t="s">
+        <v>1583</v>
+      </c>
+      <c r="J430" s="9" t="s">
+        <v>1583</v>
+      </c>
     </row>
     <row r="431" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A431" s="6" t="s">
-        <v>1582</v>
+        <v>1584</v>
       </c>
       <c r="B431" s="6" t="s">
         <v>40</v>
@@ -29087,7 +29157,7 @@
     </row>
     <row r="432" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A432" s="6" t="s">
-        <v>1583</v>
+        <v>1585</v>
       </c>
       <c r="B432" s="6" t="s">
         <v>40</v>
@@ -29113,7 +29183,7 @@
     </row>
     <row r="433" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A433" s="6" t="s">
-        <v>1584</v>
+        <v>1586</v>
       </c>
       <c r="B433" s="6" t="s">
         <v>40</v>
@@ -29139,7 +29209,7 @@
     </row>
     <row r="434" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A434" s="6" t="s">
-        <v>1585</v>
+        <v>1587</v>
       </c>
       <c r="B434" s="6" t="s">
         <v>40</v>
@@ -29165,7 +29235,7 @@
     </row>
     <row r="435" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A435" s="6" t="s">
-        <v>1586</v>
+        <v>1588</v>
       </c>
       <c r="B435" s="6" t="s">
         <v>40</v>
@@ -29191,7 +29261,7 @@
     </row>
     <row r="436" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A436" s="6" t="s">
-        <v>1587</v>
+        <v>1589</v>
       </c>
       <c r="B436" s="6" t="s">
         <v>40</v>
@@ -29217,7 +29287,7 @@
     </row>
     <row r="437" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A437" s="6" t="s">
-        <v>1588</v>
+        <v>1590</v>
       </c>
       <c r="B437" s="6" t="s">
         <v>40</v>
@@ -29243,7 +29313,7 @@
     </row>
     <row r="438" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A438" s="6" t="s">
-        <v>1589</v>
+        <v>1591</v>
       </c>
       <c r="B438" s="6" t="s">
         <v>40</v>
@@ -29269,7 +29339,7 @@
     </row>
     <row r="439" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A439" s="6" t="s">
-        <v>1590</v>
+        <v>1592</v>
       </c>
       <c r="B439" s="6" t="s">
         <v>11</v>
@@ -29287,21 +29357,21 @@
         <v>40</v>
       </c>
       <c r="G439" s="9" t="s">
-        <v>1591</v>
+        <v>1593</v>
       </c>
       <c r="H439" s="9" t="s">
-        <v>1591</v>
+        <v>1593</v>
       </c>
       <c r="I439" s="9" t="s">
-        <v>1591</v>
+        <v>1593</v>
       </c>
       <c r="J439" s="9" t="s">
-        <v>1592</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="440" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A440" s="6" t="s">
-        <v>1593</v>
+        <v>1595</v>
       </c>
       <c r="B440" s="6" t="s">
         <v>11</v>
@@ -29319,21 +29389,21 @@
         <v>40</v>
       </c>
       <c r="G440" s="9" t="s">
-        <v>1594</v>
+        <v>1596</v>
       </c>
       <c r="H440" s="9" t="s">
-        <v>1594</v>
+        <v>1596</v>
       </c>
       <c r="I440" s="9" t="s">
-        <v>1594</v>
+        <v>1596</v>
       </c>
       <c r="J440" s="9" t="s">
-        <v>1595</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="441" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A441" s="6" t="s">
-        <v>1596</v>
+        <v>1598</v>
       </c>
       <c r="B441" s="6" t="s">
         <v>40</v>
@@ -29359,7 +29429,7 @@
     </row>
     <row r="442" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A442" s="6" t="s">
-        <v>1597</v>
+        <v>1599</v>
       </c>
       <c r="B442" s="6" t="s">
         <v>11</v>
@@ -29377,21 +29447,21 @@
         <v>40</v>
       </c>
       <c r="G442" s="9" t="s">
-        <v>1598</v>
+        <v>1600</v>
       </c>
       <c r="H442" s="9" t="s">
-        <v>1598</v>
+        <v>1600</v>
       </c>
       <c r="I442" s="9" t="s">
-        <v>1598</v>
+        <v>1600</v>
       </c>
       <c r="J442" s="9" t="s">
-        <v>1599</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="443" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A443" s="6" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="B443" s="6" t="s">
         <v>11</v>
@@ -29409,21 +29479,21 @@
         <v>11</v>
       </c>
       <c r="G443" s="9" t="s">
-        <v>1601</v>
+        <v>1603</v>
       </c>
       <c r="H443" s="9" t="s">
-        <v>1601</v>
+        <v>1603</v>
       </c>
       <c r="I443" s="9" t="s">
-        <v>1601</v>
+        <v>1603</v>
       </c>
       <c r="J443" s="9" t="s">
-        <v>1602</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="444" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A444" s="6" t="s">
-        <v>1603</v>
+        <v>1605</v>
       </c>
       <c r="B444" s="6" t="s">
         <v>11</v>
@@ -29441,21 +29511,21 @@
         <v>11</v>
       </c>
       <c r="G444" s="9" t="s">
-        <v>1604</v>
+        <v>1606</v>
       </c>
       <c r="H444" s="9" t="s">
-        <v>1604</v>
+        <v>1606</v>
       </c>
       <c r="I444" s="9" t="s">
-        <v>1604</v>
+        <v>1606</v>
       </c>
       <c r="J444" s="9" t="s">
-        <v>1605</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="445" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A445" s="6" t="s">
-        <v>1606</v>
+        <v>1608</v>
       </c>
       <c r="B445" s="6" t="s">
         <v>40</v>
@@ -29481,7 +29551,7 @@
     </row>
     <row r="446" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A446" s="6" t="s">
-        <v>1607</v>
+        <v>1609</v>
       </c>
       <c r="B446" s="6" t="s">
         <v>40</v>
@@ -29507,7 +29577,7 @@
     </row>
     <row r="447" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A447" s="6" t="s">
-        <v>1608</v>
+        <v>1610</v>
       </c>
       <c r="B447" s="6" t="s">
         <v>40</v>
@@ -29533,7 +29603,7 @@
     </row>
     <row r="448" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A448" s="6" t="s">
-        <v>1609</v>
+        <v>1611</v>
       </c>
       <c r="B448" s="6" t="s">
         <v>40</v>
@@ -29559,7 +29629,7 @@
     </row>
     <row r="449" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A449" s="6" t="s">
-        <v>1610</v>
+        <v>1612</v>
       </c>
       <c r="B449" s="6" t="s">
         <v>40</v>
@@ -29585,7 +29655,7 @@
     </row>
     <row r="450" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A450" s="6" t="s">
-        <v>1611</v>
+        <v>1613</v>
       </c>
       <c r="B450" s="6" t="s">
         <v>40</v>
@@ -29611,7 +29681,7 @@
     </row>
     <row r="451" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A451" s="6" t="s">
-        <v>1612</v>
+        <v>1614</v>
       </c>
       <c r="B451" s="6" t="s">
         <v>40</v>
@@ -29637,7 +29707,7 @@
     </row>
     <row r="452" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A452" s="6" t="s">
-        <v>1613</v>
+        <v>1615</v>
       </c>
       <c r="B452" s="6" t="s">
         <v>40</v>
@@ -29663,7 +29733,7 @@
     </row>
     <row r="453" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A453" s="6" t="s">
-        <v>1614</v>
+        <v>1616</v>
       </c>
       <c r="B453" s="6" t="s">
         <v>11</v>
@@ -29681,21 +29751,21 @@
         <v>11</v>
       </c>
       <c r="G453" s="9" t="s">
-        <v>1615</v>
+        <v>1617</v>
       </c>
       <c r="H453" s="9" t="s">
-        <v>1615</v>
+        <v>1617</v>
       </c>
       <c r="I453" s="9" t="s">
-        <v>1615</v>
+        <v>1617</v>
       </c>
       <c r="J453" s="9" t="s">
-        <v>1616</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="454" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A454" s="6" t="s">
-        <v>1617</v>
+        <v>1619</v>
       </c>
       <c r="B454" s="6" t="s">
         <v>40</v>
@@ -29721,7 +29791,7 @@
     </row>
     <row r="455" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A455" s="6" t="s">
-        <v>1618</v>
+        <v>1620</v>
       </c>
       <c r="B455" s="6" t="s">
         <v>11</v>
@@ -29739,21 +29809,21 @@
         <v>11</v>
       </c>
       <c r="G455" s="9" t="s">
-        <v>1619</v>
+        <v>1621</v>
       </c>
       <c r="H455" s="9" t="s">
-        <v>1619</v>
+        <v>1621</v>
       </c>
       <c r="I455" s="9" t="s">
-        <v>1619</v>
+        <v>1621</v>
       </c>
       <c r="J455" s="9" t="s">
-        <v>1620</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="456" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A456" s="6" t="s">
-        <v>1621</v>
+        <v>1623</v>
       </c>
       <c r="B456" s="6" t="s">
         <v>40</v>
@@ -29779,7 +29849,7 @@
     </row>
     <row r="457" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A457" s="6" t="s">
-        <v>1622</v>
+        <v>1624</v>
       </c>
       <c r="B457" s="6" t="s">
         <v>40</v>
@@ -29805,7 +29875,7 @@
     </row>
     <row r="458" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A458" s="6" t="s">
-        <v>1623</v>
+        <v>1625</v>
       </c>
       <c r="B458" s="6" t="s">
         <v>40</v>
@@ -29831,7 +29901,7 @@
     </row>
     <row r="459" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A459" s="6" t="s">
-        <v>1624</v>
+        <v>1626</v>
       </c>
       <c r="B459" s="6" t="s">
         <v>40</v>
@@ -29857,7 +29927,7 @@
     </row>
     <row r="460" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A460" s="6" t="s">
-        <v>1625</v>
+        <v>1627</v>
       </c>
       <c r="B460" s="6" t="s">
         <v>11</v>
@@ -29875,21 +29945,21 @@
         <v>11</v>
       </c>
       <c r="G460" s="9" t="s">
-        <v>1626</v>
+        <v>1628</v>
       </c>
       <c r="H460" s="9" t="s">
-        <v>1626</v>
+        <v>1628</v>
       </c>
       <c r="I460" s="9" t="s">
-        <v>1626</v>
+        <v>1628</v>
       </c>
       <c r="J460" s="26" t="s">
-        <v>1627</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="461" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A461" s="6" t="s">
-        <v>1628</v>
+        <v>1630</v>
       </c>
       <c r="B461" s="6" t="s">
         <v>11</v>
@@ -29907,21 +29977,21 @@
         <v>11</v>
       </c>
       <c r="G461" s="9" t="s">
-        <v>1629</v>
+        <v>1631</v>
       </c>
       <c r="H461" s="9" t="s">
-        <v>1629</v>
+        <v>1631</v>
       </c>
       <c r="I461" s="9" t="s">
-        <v>1629</v>
+        <v>1631</v>
       </c>
       <c r="J461" s="26" t="s">
-        <v>1630</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="462" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A462" s="6" t="s">
-        <v>1631</v>
+        <v>1633</v>
       </c>
       <c r="B462" s="6" t="s">
         <v>40</v>
@@ -29947,7 +30017,7 @@
     </row>
     <row r="463" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A463" s="6" t="s">
-        <v>1632</v>
+        <v>1634</v>
       </c>
       <c r="B463" s="6" t="s">
         <v>11</v>
@@ -29965,21 +30035,21 @@
         <v>11</v>
       </c>
       <c r="G463" s="9" t="s">
-        <v>1633</v>
+        <v>1635</v>
       </c>
       <c r="H463" s="9" t="s">
-        <v>1633</v>
+        <v>1635</v>
       </c>
       <c r="I463" s="9" t="s">
-        <v>1633</v>
+        <v>1635</v>
       </c>
       <c r="J463" s="26" t="s">
-        <v>1634</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="464" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A464" s="6" t="s">
-        <v>1635</v>
+        <v>1637</v>
       </c>
       <c r="B464" s="6" t="s">
         <v>40</v>
@@ -30005,7 +30075,7 @@
     </row>
     <row r="465" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A465" s="6" t="s">
-        <v>1636</v>
+        <v>1638</v>
       </c>
       <c r="B465" s="6" t="s">
         <v>40</v>
@@ -30031,7 +30101,7 @@
     </row>
     <row r="466" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A466" s="6" t="s">
-        <v>1637</v>
+        <v>1639</v>
       </c>
       <c r="B466" s="6" t="s">
         <v>11</v>
@@ -30049,21 +30119,21 @@
         <v>40</v>
       </c>
       <c r="G466" s="9" t="s">
-        <v>1638</v>
+        <v>1640</v>
       </c>
       <c r="H466" s="9" t="s">
-        <v>1638</v>
+        <v>1640</v>
       </c>
       <c r="I466" s="9" t="s">
-        <v>1638</v>
+        <v>1640</v>
       </c>
       <c r="J466" s="9" t="s">
-        <v>1639</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="467" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A467" s="6" t="s">
-        <v>1640</v>
+        <v>1642</v>
       </c>
       <c r="B467" s="6" t="s">
         <v>40</v>
@@ -30089,7 +30159,7 @@
     </row>
     <row r="468" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A468" s="6" t="s">
-        <v>1641</v>
+        <v>1643</v>
       </c>
       <c r="B468" s="6" t="s">
         <v>40</v>
@@ -30107,21 +30177,21 @@
         <v>11</v>
       </c>
       <c r="G468" s="9" t="s">
-        <v>1642</v>
+        <v>1644</v>
       </c>
       <c r="H468" s="9" t="s">
-        <v>1642</v>
+        <v>1644</v>
       </c>
       <c r="I468" s="9" t="s">
-        <v>1642</v>
+        <v>1644</v>
       </c>
       <c r="J468" s="9" t="s">
-        <v>1643</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="469" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A469" s="6" t="s">
-        <v>1644</v>
+        <v>1646</v>
       </c>
       <c r="B469" s="6" t="s">
         <v>11</v>
@@ -30139,21 +30209,21 @@
         <v>11</v>
       </c>
       <c r="G469" s="9" t="s">
-        <v>1645</v>
+        <v>1647</v>
       </c>
       <c r="H469" s="9" t="s">
-        <v>1645</v>
+        <v>1647</v>
       </c>
       <c r="I469" s="9" t="s">
-        <v>1645</v>
+        <v>1647</v>
       </c>
       <c r="J469" s="9" t="s">
-        <v>1646</v>
+        <v>1648</v>
       </c>
     </row>
     <row r="470" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A470" s="6" t="s">
-        <v>1647</v>
+        <v>1649</v>
       </c>
       <c r="B470" s="6" t="s">
         <v>11</v>
@@ -30171,21 +30241,21 @@
         <v>11</v>
       </c>
       <c r="G470" s="9" t="s">
-        <v>1648</v>
+        <v>1650</v>
       </c>
       <c r="H470" s="9" t="s">
-        <v>1648</v>
+        <v>1650</v>
       </c>
       <c r="I470" s="9" t="s">
-        <v>1648</v>
+        <v>1650</v>
       </c>
       <c r="J470" s="9" t="s">
-        <v>1649</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="471" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A471" s="6" t="s">
-        <v>1650</v>
+        <v>1652</v>
       </c>
       <c r="B471" s="6" t="s">
         <v>11</v>
@@ -30203,21 +30273,21 @@
         <v>11</v>
       </c>
       <c r="G471" s="9" t="s">
-        <v>1651</v>
+        <v>1653</v>
       </c>
       <c r="H471" s="9" t="s">
-        <v>1651</v>
+        <v>1653</v>
       </c>
       <c r="I471" s="9" t="s">
-        <v>1651</v>
+        <v>1653</v>
       </c>
       <c r="J471" s="26" t="s">
-        <v>1652</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="472" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A472" s="6" t="s">
-        <v>1653</v>
+        <v>1655</v>
       </c>
       <c r="B472" s="6" t="s">
         <v>11</v>
@@ -30235,21 +30305,21 @@
         <v>11</v>
       </c>
       <c r="G472" s="9" t="s">
-        <v>1654</v>
+        <v>1656</v>
       </c>
       <c r="H472" s="9" t="s">
-        <v>1654</v>
+        <v>1656</v>
       </c>
       <c r="I472" s="9" t="s">
-        <v>1654</v>
+        <v>1656</v>
       </c>
       <c r="J472" s="26" t="s">
-        <v>1655</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="473" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A473" s="6" t="s">
-        <v>1656</v>
+        <v>1658</v>
       </c>
       <c r="B473" s="6" t="s">
         <v>11</v>
@@ -30267,21 +30337,21 @@
         <v>11</v>
       </c>
       <c r="G473" s="9" t="s">
-        <v>1657</v>
+        <v>1659</v>
       </c>
       <c r="H473" s="9" t="s">
-        <v>1657</v>
+        <v>1659</v>
       </c>
       <c r="I473" s="9" t="s">
-        <v>1657</v>
+        <v>1659</v>
       </c>
       <c r="J473" s="26" t="s">
-        <v>1658</v>
+        <v>1660</v>
       </c>
     </row>
     <row r="474" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A474" s="6" t="s">
-        <v>1659</v>
+        <v>1661</v>
       </c>
       <c r="B474" s="6" t="s">
         <v>40</v>
@@ -30305,7 +30375,7 @@
     </row>
     <row r="475" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A475" s="6" t="s">
-        <v>1660</v>
+        <v>1662</v>
       </c>
       <c r="B475" s="6" t="s">
         <v>40</v>
@@ -30329,7 +30399,7 @@
     </row>
     <row r="476" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A476" s="6" t="s">
-        <v>1661</v>
+        <v>1663</v>
       </c>
       <c r="B476" s="6" t="s">
         <v>40</v>
@@ -30353,7 +30423,7 @@
     </row>
     <row r="477" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A477" s="6" t="s">
-        <v>1662</v>
+        <v>1664</v>
       </c>
       <c r="B477" s="6" t="s">
         <v>40</v>
@@ -30377,7 +30447,7 @@
     </row>
     <row r="478" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A478" s="6" t="s">
-        <v>1663</v>
+        <v>1665</v>
       </c>
       <c r="B478" s="6" t="s">
         <v>40</v>
@@ -30401,7 +30471,7 @@
     </row>
     <row r="479" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A479" s="6" t="s">
-        <v>1664</v>
+        <v>1666</v>
       </c>
       <c r="B479" s="6" t="s">
         <v>40</v>
@@ -30425,7 +30495,7 @@
     </row>
     <row r="480" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A480" s="6" t="s">
-        <v>1665</v>
+        <v>1667</v>
       </c>
       <c r="B480" s="6" t="s">
         <v>40</v>
@@ -30449,7 +30519,7 @@
     </row>
     <row r="481" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A481" s="6" t="s">
-        <v>1666</v>
+        <v>1668</v>
       </c>
       <c r="B481" s="6" t="s">
         <v>40</v>
@@ -30473,7 +30543,7 @@
     </row>
     <row r="482" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A482" s="6" t="s">
-        <v>1667</v>
+        <v>1669</v>
       </c>
       <c r="B482" s="6" t="s">
         <v>40</v>
@@ -30497,7 +30567,7 @@
     </row>
     <row r="483" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A483" s="6" t="s">
-        <v>1668</v>
+        <v>1670</v>
       </c>
       <c r="B483" s="6" t="s">
         <v>40</v>
@@ -30521,7 +30591,7 @@
     </row>
     <row r="484" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A484" s="6" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="B484" s="6" t="s">
         <v>40</v>
@@ -30545,7 +30615,7 @@
     </row>
     <row r="485" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A485" s="6" t="s">
-        <v>1670</v>
+        <v>1672</v>
       </c>
       <c r="B485" s="6" t="s">
         <v>40</v>
@@ -30569,7 +30639,7 @@
     </row>
     <row r="486" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A486" s="6" t="s">
-        <v>1671</v>
+        <v>1673</v>
       </c>
       <c r="B486" s="6" t="s">
         <v>40</v>
@@ -30593,7 +30663,7 @@
     </row>
     <row r="487" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A487" s="6" t="s">
-        <v>1672</v>
+        <v>1674</v>
       </c>
       <c r="B487" s="6" t="s">
         <v>40</v>
@@ -30617,7 +30687,7 @@
     </row>
     <row r="488" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A488" s="6" t="s">
-        <v>1673</v>
+        <v>1675</v>
       </c>
       <c r="B488" s="6" t="s">
         <v>40</v>
@@ -30641,7 +30711,7 @@
     </row>
     <row r="489" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A489" s="6" t="s">
-        <v>1674</v>
+        <v>1676</v>
       </c>
       <c r="B489" s="6" t="s">
         <v>40</v>
@@ -30665,7 +30735,7 @@
     </row>
     <row r="490" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A490" s="6" t="s">
-        <v>1675</v>
+        <v>1677</v>
       </c>
       <c r="B490" s="6" t="s">
         <v>40</v>
@@ -30689,7 +30759,7 @@
     </row>
     <row r="491" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A491" s="6" t="s">
-        <v>1676</v>
+        <v>1678</v>
       </c>
       <c r="B491" s="6" t="s">
         <v>40</v>
@@ -30713,7 +30783,7 @@
     </row>
     <row r="492" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A492" s="6" t="s">
-        <v>1677</v>
+        <v>1679</v>
       </c>
       <c r="B492" s="6" t="s">
         <v>40</v>
@@ -30737,7 +30807,7 @@
     </row>
     <row r="493" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A493" s="6" t="s">
-        <v>1678</v>
+        <v>1680</v>
       </c>
       <c r="B493" s="6" t="s">
         <v>40</v>
@@ -30761,7 +30831,7 @@
     </row>
     <row r="494" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A494" s="6" t="s">
-        <v>1679</v>
+        <v>1681</v>
       </c>
       <c r="B494" s="6" t="s">
         <v>40</v>
@@ -30785,7 +30855,7 @@
     </row>
     <row r="495" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A495" s="6" t="s">
-        <v>1680</v>
+        <v>1682</v>
       </c>
       <c r="B495" s="6" t="s">
         <v>40</v>
@@ -30809,7 +30879,7 @@
     </row>
     <row r="496" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A496" s="6" t="s">
-        <v>1681</v>
+        <v>1683</v>
       </c>
       <c r="B496" s="6" t="s">
         <v>40</v>
@@ -30833,7 +30903,7 @@
     </row>
     <row r="497" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A497" s="6" t="s">
-        <v>1682</v>
+        <v>1684</v>
       </c>
       <c r="B497" s="6" t="s">
         <v>40</v>
@@ -30857,7 +30927,7 @@
     </row>
     <row r="498" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A498" s="6" t="s">
-        <v>1683</v>
+        <v>1685</v>
       </c>
       <c r="B498" s="6" t="s">
         <v>40</v>
@@ -30881,7 +30951,7 @@
     </row>
     <row r="499" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A499" s="6" t="s">
-        <v>1684</v>
+        <v>1686</v>
       </c>
       <c r="B499" s="6" t="s">
         <v>40</v>
@@ -30905,7 +30975,7 @@
     </row>
     <row r="500" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A500" s="6" t="s">
-        <v>1685</v>
+        <v>1687</v>
       </c>
       <c r="B500" s="6" t="s">
         <v>40</v>
@@ -30929,7 +30999,7 @@
     </row>
     <row r="501" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A501" s="6" t="s">
-        <v>1686</v>
+        <v>1688</v>
       </c>
       <c r="B501" s="6" t="s">
         <v>40</v>
@@ -30953,7 +31023,7 @@
     </row>
     <row r="502" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A502" s="6" t="s">
-        <v>1687</v>
+        <v>1689</v>
       </c>
       <c r="B502" s="6" t="s">
         <v>40</v>
@@ -30977,7 +31047,7 @@
     </row>
     <row r="503" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A503" s="6" t="s">
-        <v>1688</v>
+        <v>1690</v>
       </c>
       <c r="B503" s="6" t="s">
         <v>40</v>
@@ -31001,7 +31071,7 @@
     </row>
     <row r="504" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A504" s="6" t="s">
-        <v>1689</v>
+        <v>1691</v>
       </c>
       <c r="B504" s="6" t="s">
         <v>40</v>
@@ -31025,7 +31095,7 @@
     </row>
     <row r="505" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A505" s="6" t="s">
-        <v>1690</v>
+        <v>1692</v>
       </c>
       <c r="B505" s="6" t="s">
         <v>40</v>
@@ -31049,7 +31119,7 @@
     </row>
     <row r="506" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A506" s="6" t="s">
-        <v>1691</v>
+        <v>1693</v>
       </c>
       <c r="B506" s="6" t="s">
         <v>40</v>
@@ -31073,7 +31143,7 @@
     </row>
     <row r="507" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A507" s="6" t="s">
-        <v>1692</v>
+        <v>1694</v>
       </c>
       <c r="B507" s="6" t="s">
         <v>40</v>
@@ -31097,7 +31167,7 @@
     </row>
     <row r="508" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A508" s="6" t="s">
-        <v>1693</v>
+        <v>1695</v>
       </c>
       <c r="B508" s="6" t="s">
         <v>40</v>
@@ -31121,7 +31191,7 @@
     </row>
     <row r="509" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A509" s="6" t="s">
-        <v>1694</v>
+        <v>1696</v>
       </c>
       <c r="B509" s="6" t="s">
         <v>40</v>
@@ -31145,7 +31215,7 @@
     </row>
     <row r="510" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A510" s="6" t="s">
-        <v>1695</v>
+        <v>1697</v>
       </c>
       <c r="B510" s="6" t="s">
         <v>40</v>
@@ -31169,7 +31239,7 @@
     </row>
     <row r="511" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A511" s="6" t="s">
-        <v>1696</v>
+        <v>1698</v>
       </c>
       <c r="B511" s="6" t="s">
         <v>40</v>
@@ -31193,7 +31263,7 @@
     </row>
     <row r="512" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A512" s="6" t="s">
-        <v>1697</v>
+        <v>1699</v>
       </c>
       <c r="B512" s="6" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Fixed ssl not included. Added RE armors
</commit_message>
<xml_diff>
--- a/scripts/MHW_Armor_Data.xlsx
+++ b/scripts/MHW_Armor_Data.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4764" uniqueCount="1700">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4770" uniqueCount="1702">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -14013,15 +14013,629 @@
     <t xml:space="preserve">428</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Rajang </t>
+    <t xml:space="preserve">Rajang α+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">429</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rajang β+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">430</t>
+  </si>
+  <si>
+    <t xml:space="preserve">431</t>
+  </si>
+  <si>
+    <t xml:space="preserve">432</t>
+  </si>
+  <si>
+    <t xml:space="preserve">433</t>
+  </si>
+  <si>
+    <t xml:space="preserve">434</t>
+  </si>
+  <si>
+    <t xml:space="preserve">435</t>
+  </si>
+  <si>
+    <t xml:space="preserve">436</t>
+  </si>
+  <si>
+    <t xml:space="preserve">437</t>
+  </si>
+  <si>
+    <t xml:space="preserve">438</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sealed Dragon Cloth α+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">EX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">봉인의 용해포</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">α </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">439</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wyverian Ears α+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">EX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">용인족의 귀</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">α </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">440</t>
+  </si>
+  <si>
+    <t xml:space="preserve">441</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duffel Penguin Mask α+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">EX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">껴입기펭귄페이크</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">α </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">442</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lunastra α+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">EX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">엠프리스</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">α</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">443</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lunastra β+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">EX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">엠프리스</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">β</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">444</t>
+  </si>
+  <si>
+    <t xml:space="preserve">445</t>
+  </si>
+  <si>
+    <t xml:space="preserve">446</t>
+  </si>
+  <si>
+    <t xml:space="preserve">447</t>
+  </si>
+  <si>
+    <t xml:space="preserve">448</t>
+  </si>
+  <si>
+    <t xml:space="preserve">449</t>
+  </si>
+  <si>
+    <t xml:space="preserve">450</t>
+  </si>
+  <si>
+    <t xml:space="preserve">451</t>
+  </si>
+  <si>
+    <t xml:space="preserve">452</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oolong α+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">EX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">우론</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">α</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">453</t>
+  </si>
+  <si>
+    <t xml:space="preserve">454</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Astral α+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">EX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">아스트라</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">α</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">455</t>
+  </si>
+  <si>
+    <t xml:space="preserve">456</t>
+  </si>
+  <si>
+    <t xml:space="preserve">457</t>
+  </si>
+  <si>
+    <t xml:space="preserve">458</t>
+  </si>
+  <si>
+    <t xml:space="preserve">459</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oolong Layered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">【우론】의상</t>
+  </si>
+  <si>
+    <t xml:space="preserve">460</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Astral Layered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">【아스트라】의상</t>
+  </si>
+  <si>
+    <t xml:space="preserve">461</t>
+  </si>
+  <si>
+    <t xml:space="preserve">462</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thermae Layered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">【테르마이】의상</t>
+  </si>
+  <si>
+    <t xml:space="preserve">463</t>
+  </si>
+  <si>
+    <t xml:space="preserve">464</t>
+  </si>
+  <si>
+    <t xml:space="preserve">465</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pearlspring α+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">EX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">은천원숭이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">α </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">466</t>
+  </si>
+  <si>
+    <t xml:space="preserve">467</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buff Body α+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">EX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">머슬보디</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">α </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">468</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brute Tigrex α+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">EX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">렉스로어</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">α</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">469</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brute Tigrex β+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">EX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">렉스로어</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">β</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">470</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guardian α+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">가디언</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">α</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">471</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yukumo Layered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">【유쿠모】의상</t>
+  </si>
+  <si>
+    <t xml:space="preserve">472</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silver Knight Layered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">【은기사】의상</t>
+  </si>
+  <si>
+    <t xml:space="preserve">473</t>
+  </si>
+  <si>
+    <t xml:space="preserve">474</t>
+  </si>
+  <si>
+    <t xml:space="preserve">475</t>
+  </si>
+  <si>
+    <t xml:space="preserve">476</t>
+  </si>
+  <si>
+    <t xml:space="preserve">477</t>
+  </si>
+  <si>
+    <t xml:space="preserve">478</t>
+  </si>
+  <si>
+    <t xml:space="preserve">479</t>
+  </si>
+  <si>
+    <t xml:space="preserve">480</t>
+  </si>
+  <si>
+    <t xml:space="preserve">481</t>
+  </si>
+  <si>
+    <t xml:space="preserve">482</t>
+  </si>
+  <si>
+    <t xml:space="preserve">483</t>
+  </si>
+  <si>
+    <t xml:space="preserve">484</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Leon </t>
     </r>
     <r>
       <rPr>
@@ -14034,646 +14648,28 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">429</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Rajang </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">β</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">+</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">430</t>
-  </si>
-  <si>
-    <t xml:space="preserve">431</t>
-  </si>
-  <si>
-    <t xml:space="preserve">432</t>
-  </si>
-  <si>
-    <t xml:space="preserve">433</t>
-  </si>
-  <si>
-    <t xml:space="preserve">434</t>
-  </si>
-  <si>
-    <t xml:space="preserve">435</t>
-  </si>
-  <si>
-    <t xml:space="preserve">436</t>
-  </si>
-  <si>
-    <t xml:space="preserve">437</t>
-  </si>
-  <si>
-    <t xml:space="preserve">438</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sealed Dragon Cloth α+</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">EX</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">봉인의 용해포</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">α </t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">439</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wyverian Ears α+</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">EX</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">용인족의 귀</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">α </t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">440</t>
-  </si>
-  <si>
-    <t xml:space="preserve">441</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duffel Penguin Mask α+</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">EX</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">껴입기펭귄페이크</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">α </t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">442</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lunastra α+</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">EX</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">엠프리스</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">α</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">443</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lunastra β+</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">EX</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">엠프리스</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">β</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">444</t>
-  </si>
-  <si>
-    <t xml:space="preserve">445</t>
-  </si>
-  <si>
-    <t xml:space="preserve">446</t>
-  </si>
-  <si>
-    <t xml:space="preserve">447</t>
-  </si>
-  <si>
-    <t xml:space="preserve">448</t>
-  </si>
-  <si>
-    <t xml:space="preserve">449</t>
-  </si>
-  <si>
-    <t xml:space="preserve">450</t>
-  </si>
-  <si>
-    <t xml:space="preserve">451</t>
-  </si>
-  <si>
-    <t xml:space="preserve">452</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oolong α+</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">EX</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">우론</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">α</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">453</t>
-  </si>
-  <si>
-    <t xml:space="preserve">454</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Astral α+</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">EX</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">아스트라</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">α</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">455</t>
-  </si>
-  <si>
-    <t xml:space="preserve">456</t>
-  </si>
-  <si>
-    <t xml:space="preserve">457</t>
-  </si>
-  <si>
-    <t xml:space="preserve">458</t>
-  </si>
-  <si>
-    <t xml:space="preserve">459</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oolong Layered</t>
-  </si>
-  <si>
-    <t xml:space="preserve">【우론】의상</t>
-  </si>
-  <si>
-    <t xml:space="preserve">460</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Astral Layered</t>
-  </si>
-  <si>
-    <t xml:space="preserve">【아스트라】의상</t>
-  </si>
-  <si>
-    <t xml:space="preserve">461</t>
-  </si>
-  <si>
-    <t xml:space="preserve">462</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thermae Layered</t>
-  </si>
-  <si>
-    <t xml:space="preserve">【테르마이】의상</t>
-  </si>
-  <si>
-    <t xml:space="preserve">463</t>
-  </si>
-  <si>
-    <t xml:space="preserve">464</t>
-  </si>
-  <si>
-    <t xml:space="preserve">465</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pearlspring α+</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">EX</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">은천원숭이</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">α </t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">466</t>
-  </si>
-  <si>
-    <t xml:space="preserve">467</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Buff Body α+</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">EX</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">머슬보디</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">α </t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">468</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brute Tigrex α+</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">EX</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">렉스로어</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">α</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">469</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brute Tigrex β+</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">EX</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">렉스로어</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">β</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">470</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guardian α+</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">가디언</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">α</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">471</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yukumo Layered</t>
-  </si>
-  <si>
-    <t xml:space="preserve">【유쿠모】의상</t>
-  </si>
-  <si>
-    <t xml:space="preserve">472</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Silver Knight Layered</t>
-  </si>
-  <si>
-    <t xml:space="preserve">【은기사】의상</t>
-  </si>
-  <si>
-    <t xml:space="preserve">473</t>
-  </si>
-  <si>
-    <t xml:space="preserve">474</t>
-  </si>
-  <si>
-    <t xml:space="preserve">475</t>
-  </si>
-  <si>
-    <t xml:space="preserve">476</t>
-  </si>
-  <si>
-    <t xml:space="preserve">477</t>
-  </si>
-  <si>
-    <t xml:space="preserve">478</t>
-  </si>
-  <si>
-    <t xml:space="preserve">479</t>
-  </si>
-  <si>
-    <t xml:space="preserve">480</t>
-  </si>
-  <si>
-    <t xml:space="preserve">481</t>
-  </si>
-  <si>
-    <t xml:space="preserve">482</t>
-  </si>
-  <si>
-    <t xml:space="preserve">483</t>
-  </si>
-  <si>
-    <t xml:space="preserve">484</t>
-  </si>
-  <si>
     <t xml:space="preserve">485</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Claire </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">α+</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">486</t>
@@ -14902,15 +14898,15 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Cambria"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Cambria"/>
+      <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -15132,7 +15128,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -15155,8 +15151,8 @@
   </sheetPr>
   <dimension ref="A1:M1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A421" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F430" activeCellId="0" sqref="F430"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A463" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D485" activeCellId="0" sqref="D485"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -30618,52 +30614,68 @@
         <v>1672</v>
       </c>
       <c r="B485" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C485" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D485" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="E485" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="F485" s="16" t="s">
-        <v>40</v>
+        <v>11</v>
+      </c>
+      <c r="C485" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D485" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E485" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F485" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="G485" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="J485" s="27"/>
+        <v>1673</v>
+      </c>
+      <c r="H485" s="9" t="s">
+        <v>1673</v>
+      </c>
+      <c r="I485" s="9" t="s">
+        <v>1673</v>
+      </c>
+      <c r="J485" s="9" t="s">
+        <v>1673</v>
+      </c>
     </row>
     <row r="486" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A486" s="6" t="s">
-        <v>1673</v>
+        <v>1674</v>
       </c>
       <c r="B486" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C486" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D486" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="E486" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="F486" s="16" t="s">
-        <v>40</v>
+        <v>11</v>
+      </c>
+      <c r="C486" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D486" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E486" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F486" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="G486" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="J486" s="27"/>
+        <v>1675</v>
+      </c>
+      <c r="H486" s="9" t="s">
+        <v>1675</v>
+      </c>
+      <c r="I486" s="9" t="s">
+        <v>1675</v>
+      </c>
+      <c r="J486" s="9" t="s">
+        <v>1675</v>
+      </c>
     </row>
     <row r="487" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A487" s="6" t="s">
-        <v>1674</v>
+        <v>1676</v>
       </c>
       <c r="B487" s="6" t="s">
         <v>40</v>
@@ -30687,7 +30699,7 @@
     </row>
     <row r="488" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A488" s="6" t="s">
-        <v>1675</v>
+        <v>1677</v>
       </c>
       <c r="B488" s="6" t="s">
         <v>40</v>
@@ -30711,7 +30723,7 @@
     </row>
     <row r="489" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A489" s="6" t="s">
-        <v>1676</v>
+        <v>1678</v>
       </c>
       <c r="B489" s="6" t="s">
         <v>40</v>
@@ -30735,7 +30747,7 @@
     </row>
     <row r="490" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A490" s="6" t="s">
-        <v>1677</v>
+        <v>1679</v>
       </c>
       <c r="B490" s="6" t="s">
         <v>40</v>
@@ -30759,7 +30771,7 @@
     </row>
     <row r="491" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A491" s="6" t="s">
-        <v>1678</v>
+        <v>1680</v>
       </c>
       <c r="B491" s="6" t="s">
         <v>40</v>
@@ -30783,7 +30795,7 @@
     </row>
     <row r="492" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A492" s="6" t="s">
-        <v>1679</v>
+        <v>1681</v>
       </c>
       <c r="B492" s="6" t="s">
         <v>40</v>
@@ -30807,7 +30819,7 @@
     </row>
     <row r="493" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A493" s="6" t="s">
-        <v>1680</v>
+        <v>1682</v>
       </c>
       <c r="B493" s="6" t="s">
         <v>40</v>
@@ -30831,7 +30843,7 @@
     </row>
     <row r="494" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A494" s="6" t="s">
-        <v>1681</v>
+        <v>1683</v>
       </c>
       <c r="B494" s="6" t="s">
         <v>40</v>
@@ -30855,7 +30867,7 @@
     </row>
     <row r="495" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A495" s="6" t="s">
-        <v>1682</v>
+        <v>1684</v>
       </c>
       <c r="B495" s="6" t="s">
         <v>40</v>
@@ -30879,7 +30891,7 @@
     </row>
     <row r="496" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A496" s="6" t="s">
-        <v>1683</v>
+        <v>1685</v>
       </c>
       <c r="B496" s="6" t="s">
         <v>40</v>
@@ -30903,7 +30915,7 @@
     </row>
     <row r="497" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A497" s="6" t="s">
-        <v>1684</v>
+        <v>1686</v>
       </c>
       <c r="B497" s="6" t="s">
         <v>40</v>
@@ -30927,7 +30939,7 @@
     </row>
     <row r="498" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A498" s="6" t="s">
-        <v>1685</v>
+        <v>1687</v>
       </c>
       <c r="B498" s="6" t="s">
         <v>40</v>
@@ -30951,7 +30963,7 @@
     </row>
     <row r="499" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A499" s="6" t="s">
-        <v>1686</v>
+        <v>1688</v>
       </c>
       <c r="B499" s="6" t="s">
         <v>40</v>
@@ -30975,7 +30987,7 @@
     </row>
     <row r="500" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A500" s="6" t="s">
-        <v>1687</v>
+        <v>1689</v>
       </c>
       <c r="B500" s="6" t="s">
         <v>40</v>
@@ -30999,7 +31011,7 @@
     </row>
     <row r="501" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A501" s="6" t="s">
-        <v>1688</v>
+        <v>1690</v>
       </c>
       <c r="B501" s="6" t="s">
         <v>40</v>
@@ -31023,7 +31035,7 @@
     </row>
     <row r="502" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A502" s="6" t="s">
-        <v>1689</v>
+        <v>1691</v>
       </c>
       <c r="B502" s="6" t="s">
         <v>40</v>
@@ -31047,7 +31059,7 @@
     </row>
     <row r="503" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A503" s="6" t="s">
-        <v>1690</v>
+        <v>1692</v>
       </c>
       <c r="B503" s="6" t="s">
         <v>40</v>
@@ -31071,7 +31083,7 @@
     </row>
     <row r="504" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A504" s="6" t="s">
-        <v>1691</v>
+        <v>1693</v>
       </c>
       <c r="B504" s="6" t="s">
         <v>40</v>
@@ -31095,7 +31107,7 @@
     </row>
     <row r="505" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A505" s="6" t="s">
-        <v>1692</v>
+        <v>1694</v>
       </c>
       <c r="B505" s="6" t="s">
         <v>40</v>
@@ -31119,7 +31131,7 @@
     </row>
     <row r="506" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A506" s="6" t="s">
-        <v>1693</v>
+        <v>1695</v>
       </c>
       <c r="B506" s="6" t="s">
         <v>40</v>
@@ -31143,7 +31155,7 @@
     </row>
     <row r="507" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A507" s="6" t="s">
-        <v>1694</v>
+        <v>1696</v>
       </c>
       <c r="B507" s="6" t="s">
         <v>40</v>
@@ -31167,7 +31179,7 @@
     </row>
     <row r="508" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A508" s="6" t="s">
-        <v>1695</v>
+        <v>1697</v>
       </c>
       <c r="B508" s="6" t="s">
         <v>40</v>
@@ -31191,7 +31203,7 @@
     </row>
     <row r="509" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A509" s="6" t="s">
-        <v>1696</v>
+        <v>1698</v>
       </c>
       <c r="B509" s="6" t="s">
         <v>40</v>
@@ -31215,7 +31227,7 @@
     </row>
     <row r="510" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A510" s="6" t="s">
-        <v>1697</v>
+        <v>1699</v>
       </c>
       <c r="B510" s="6" t="s">
         <v>40</v>
@@ -31239,7 +31251,7 @@
     </row>
     <row r="511" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A511" s="6" t="s">
-        <v>1698</v>
+        <v>1700</v>
       </c>
       <c r="B511" s="6" t="s">
         <v>40</v>
@@ -31263,7 +31275,7 @@
     </row>
     <row r="512" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A512" s="6" t="s">
-        <v>1699</v>
+        <v>1701</v>
       </c>
       <c r="B512" s="6" t="s">
         <v>40</v>

</xml_diff>